<commit_message>
Added DCF for MSFT, NVDA, updated ASML
</commit_message>
<xml_diff>
--- a/Portfolio Models/Airbnb.xlsx
+++ b/Portfolio Models/Airbnb.xlsx
@@ -5,38 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bina/Documents/financial-modeling/growth/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bina/Documents/financial-modeling/Portfolio Models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B679BC55-BA29-5847-A0CC-4AF8AAE6E628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{765A125B-9351-054F-A888-ED567EC93784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="22140" windowHeight="28040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'Sheet 1'!$A$106</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'Sheet 1'!$A$19</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">'Sheet 1'!$B$3:$G$3</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'Sheet 1'!$B$106:$G$106</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'Sheet 1'!$B$19:$G$19</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'Sheet 1'!$B$3:$G$3</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'Sheet 1'!$A$106</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'Sheet 1'!$A$19</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'Sheet 1'!$A$3</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">'Sheet 1'!$B$106:$G$106</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">'Sheet 1'!$B$19:$G$19</definedName>
-    <definedName name="_xlchart.v2.11" hidden="1">'Sheet 1'!$A$106</definedName>
-    <definedName name="_xlchart.v2.12" hidden="1">'Sheet 1'!$A$19</definedName>
-    <definedName name="_xlchart.v2.13" hidden="1">'Sheet 1'!$A$3</definedName>
-    <definedName name="_xlchart.v2.14" hidden="1">'Sheet 1'!$B$106:$G$106</definedName>
-    <definedName name="_xlchart.v2.15" hidden="1">'Sheet 1'!$B$19:$G$19</definedName>
-    <definedName name="_xlchart.v2.16" hidden="1">'Sheet 1'!$B$3:$G$3</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -55,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="159">
   <si>
     <t>INCOME STATEMENT (in mln.)</t>
   </si>
@@ -529,6 +507,9 @@
   </si>
   <si>
     <t>Weighted Average Cost of Capital</t>
+  </si>
+  <si>
+    <t>Gross Booking Value</t>
   </si>
 </sst>
 </file>
@@ -857,7 +838,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -894,10 +875,7 @@
     <xf numFmtId="9" fontId="12" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -925,18 +903,6 @@
     <xf numFmtId="10" fontId="12" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="37" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -956,16 +922,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="1" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -974,9 +931,6 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -993,26 +947,46 @@
     <xf numFmtId="10" fontId="1" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="10" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="10" fontId="1" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="13" fillId="3" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="13" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="167" fontId="13" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1116,7 +1090,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sheet 1'!$A$3</c:f>
+              <c:f>'Sheet 1'!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1160,7 +1134,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Sheet 1'!$B$3:$G$3</c:f>
+              <c:f>'Sheet 1'!$B$4:$G$4</c:f>
               <c:numCache>
                 <c:formatCode>#,###,,;\(#,###,,\);\ \-\ \-</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1196,7 +1170,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sheet 1'!$A$19</c:f>
+              <c:f>'Sheet 1'!$A$20</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1240,7 +1214,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Sheet 1'!$B$19:$G$19</c:f>
+              <c:f>'Sheet 1'!$B$20:$G$20</c:f>
               <c:numCache>
                 <c:formatCode>#,###,,;\(#,###,,\);\ \-\ \-</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1276,7 +1250,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sheet 1'!$A$106</c:f>
+              <c:f>'Sheet 1'!$A$107</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1320,7 +1294,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Sheet 1'!$B$106:$G$106</c:f>
+              <c:f>'Sheet 1'!$B$107:$G$107</c:f>
               <c:numCache>
                 <c:formatCode>#,###,,;\(#,###,,\);\ \-\ \-</c:formatCode>
                 <c:ptCount val="6"/>
@@ -2063,13 +2037,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>812800</xdr:colOff>
-      <xdr:row>65</xdr:row>
+      <xdr:row>66</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2096,179 +2070,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet 1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="3">
-          <cell r="A3" t="str">
-            <v>Revenue</v>
-          </cell>
-          <cell r="B3">
-            <v>73000</v>
-          </cell>
-          <cell r="C3">
-            <v>14742000</v>
-          </cell>
-          <cell r="D3">
-            <v>111943000</v>
-          </cell>
-          <cell r="E3">
-            <v>116744000</v>
-          </cell>
-          <cell r="F3">
-            <v>204242000</v>
-          </cell>
-          <cell r="G3">
-            <v>413256000</v>
-          </cell>
-          <cell r="H3">
-            <v>2013496000</v>
-          </cell>
-          <cell r="I3">
-            <v>3198356000</v>
-          </cell>
-          <cell r="J3">
-            <v>4046025000</v>
-          </cell>
-          <cell r="K3">
-            <v>7000132000</v>
-          </cell>
-          <cell r="L3">
-            <v>11758751000</v>
-          </cell>
-          <cell r="M3">
-            <v>21461268000</v>
-          </cell>
-          <cell r="N3">
-            <v>24578000000</v>
-          </cell>
-          <cell r="O3">
-            <v>31536000000</v>
-          </cell>
-          <cell r="P3">
-            <v>53823000000</v>
-          </cell>
-          <cell r="Q3">
-            <v>81462000000</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="A19" t="str">
-            <v>EBITDA</v>
-          </cell>
-          <cell r="B19">
-            <v>-73403000</v>
-          </cell>
-          <cell r="C19">
-            <v>-74781000</v>
-          </cell>
-          <cell r="D19">
-            <v>-46243000</v>
-          </cell>
-          <cell r="E19">
-            <v>-142540000</v>
-          </cell>
-          <cell r="F19">
-            <v>-236960000</v>
-          </cell>
-          <cell r="G19">
-            <v>-366998000</v>
-          </cell>
-          <cell r="H19">
-            <v>67591000</v>
-          </cell>
-          <cell r="I19">
-            <v>48181000</v>
-          </cell>
-          <cell r="J19">
-            <v>-334183000</v>
-          </cell>
-          <cell r="K19">
-            <v>497693000</v>
-          </cell>
-          <cell r="L19">
-            <v>177408000</v>
-          </cell>
-          <cell r="M19">
-            <v>1645867000</v>
-          </cell>
-          <cell r="N19">
-            <v>2087000000</v>
-          </cell>
-          <cell r="O19">
-            <v>4052000000</v>
-          </cell>
-          <cell r="P19">
-            <v>9500000000</v>
-          </cell>
-          <cell r="Q19">
-            <v>17626000000</v>
-          </cell>
-        </row>
-        <row r="106">
-          <cell r="A106" t="str">
-            <v>Free Cash Flow</v>
-          </cell>
-          <cell r="B106">
-            <v>-63271000</v>
-          </cell>
-          <cell r="C106">
-            <v>-62042000</v>
-          </cell>
-          <cell r="D106">
-            <v>-92709000</v>
-          </cell>
-          <cell r="E106">
-            <v>-168020000</v>
-          </cell>
-          <cell r="F106">
-            <v>-312260000</v>
-          </cell>
-          <cell r="G106">
-            <v>-505309000</v>
-          </cell>
-          <cell r="H106">
-            <v>-6230000</v>
-          </cell>
-          <cell r="I106">
-            <v>-1027222000</v>
-          </cell>
-          <cell r="J106">
-            <v>-2159349000</v>
-          </cell>
-          <cell r="K106">
-            <v>-1564300000</v>
-          </cell>
-          <cell r="L106">
-            <v>-4142008000</v>
-          </cell>
-          <cell r="M106">
-            <v>-221714000</v>
-          </cell>
-          <cell r="N106">
-            <v>968000000</v>
-          </cell>
-          <cell r="O106">
-            <v>2701000000</v>
-          </cell>
-          <cell r="P106">
-            <v>3483000000</v>
-          </cell>
-          <cell r="Q106">
-            <v>7561000000</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2568,13 +2369,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AN118"/>
+  <dimension ref="A1:AL119"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="G61" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J99" sqref="J99"/>
+      <selection pane="bottomRight" activeCell="M78" sqref="M78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2585,7 +2386,7 @@
     <col min="13" max="16" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:38" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>94</v>
       </c>
@@ -2623,7 +2424,7 @@
         <v>2027</v>
       </c>
     </row>
-    <row r="2" spans="1:40" ht="21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:38" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -2661,989 +2462,1006 @@
       <c r="O2" s="9"/>
       <c r="P2" s="9"/>
     </row>
-    <row r="3" spans="1:40" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:38" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B3" s="32">
+        <v>13900</v>
+      </c>
+      <c r="C3" s="32">
+        <v>20970</v>
+      </c>
+      <c r="D3" s="32">
+        <v>29400</v>
+      </c>
+      <c r="E3" s="32">
+        <v>23890</v>
+      </c>
+      <c r="F3" s="32">
+        <v>46880</v>
+      </c>
+      <c r="G3" s="32">
+        <v>63200</v>
+      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="32"/>
+      <c r="R3" s="32"/>
+      <c r="S3" s="32"/>
+      <c r="T3" s="32"/>
+      <c r="U3" s="32"/>
+      <c r="V3" s="32"/>
+      <c r="W3" s="32"/>
+      <c r="X3" s="32"/>
+      <c r="Y3" s="32"/>
+      <c r="Z3" s="32"/>
+      <c r="AA3" s="32"/>
+      <c r="AB3" s="32"/>
+      <c r="AC3" s="32"/>
+      <c r="AD3" s="1"/>
+      <c r="AE3" s="1"/>
+      <c r="AF3" s="1"/>
+      <c r="AG3" s="1"/>
+      <c r="AH3" s="1"/>
+    </row>
+    <row r="4" spans="1:38" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B4" s="1">
         <v>2561721000</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C4" s="1">
         <v>3651985000</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D4" s="1">
         <v>4805239000</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E4" s="1">
         <v>3378199000</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F4" s="1">
         <v>5991760000</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G4" s="1">
         <v>8399000000</v>
       </c>
-      <c r="H3" s="15">
+      <c r="H4" s="15">
         <v>9600000000</v>
       </c>
-      <c r="I3" s="15">
+      <c r="I4" s="15">
         <v>11050000000</v>
       </c>
-      <c r="J3" s="15">
+      <c r="J4" s="15">
         <v>12900000000</v>
       </c>
-      <c r="K3" s="15">
+      <c r="K4" s="15">
         <v>14592000000</v>
       </c>
-      <c r="L3" s="15">
+      <c r="L4" s="15">
         <v>16651000000</v>
       </c>
-      <c r="M3" s="26" t="s">
+      <c r="M4" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="N3" s="27" t="s">
+      <c r="N4" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="O3" s="27" t="s">
+      <c r="O4" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="P3" s="28" t="s">
+      <c r="P4" s="25" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:40" ht="19" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+    <row r="5" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="18">
-        <f>(C3/B3)-1</f>
+      <c r="B5" s="1"/>
+      <c r="C5" s="18">
+        <f>(C4/B4)-1</f>
         <v>0.42559825991979605</v>
       </c>
-      <c r="D4" s="18">
-        <f>(D3/C3)-1</f>
+      <c r="D5" s="18">
+        <f>(D4/C4)-1</f>
         <v>0.31578826309527552</v>
       </c>
-      <c r="E4" s="18">
-        <f>(E3/D3)-1</f>
+      <c r="E5" s="18">
+        <f>(E4/D4)-1</f>
         <v>-0.29697586321929048</v>
       </c>
-      <c r="F4" s="18">
-        <f t="shared" ref="F4:J4" si="0">(F3/E3)-1</f>
+      <c r="F5" s="18">
+        <f t="shared" ref="F5:J5" si="0">(F4/E4)-1</f>
         <v>0.77365513399299446</v>
       </c>
-      <c r="G4" s="18">
+      <c r="G5" s="18">
         <f t="shared" si="0"/>
         <v>0.40175841488978192</v>
       </c>
-      <c r="H4" s="16">
+      <c r="H5" s="16">
         <f t="shared" si="0"/>
         <v>0.14299321347779492</v>
       </c>
-      <c r="I4" s="16">
+      <c r="I5" s="16">
         <f t="shared" si="0"/>
         <v>0.15104166666666674</v>
       </c>
-      <c r="J4" s="16">
+      <c r="J5" s="16">
         <f t="shared" si="0"/>
         <v>0.16742081447963808</v>
       </c>
-      <c r="K4" s="16">
-        <f t="shared" ref="K4" si="1">(K3/J3)-1</f>
+      <c r="K5" s="16">
+        <f t="shared" ref="K5" si="1">(K4/J4)-1</f>
         <v>0.13116279069767445</v>
       </c>
-      <c r="L4" s="16">
-        <f t="shared" ref="L4" si="2">(L3/K3)-1</f>
+      <c r="L5" s="16">
+        <f t="shared" ref="L5" si="2">(L4/K4)-1</f>
         <v>0.1411047149122806</v>
       </c>
-      <c r="M4" s="19">
-        <f>(G4+F4+E4)/3</f>
+      <c r="M5" s="19">
+        <f>(G5+F5+E5)/3</f>
         <v>0.29281256188782862</v>
       </c>
-      <c r="N4" s="20">
-        <f>(G20+F20+E20)/3</f>
+      <c r="N5" s="20">
+        <f>(G21+F21+E21)/3</f>
         <v>6.5927165252214168</v>
       </c>
-      <c r="O4" s="20">
-        <f>(G29+F29+E29)/3</f>
+      <c r="O5" s="20">
+        <f>(G30+F30+E30)/3</f>
         <v>-0.50056919516481246</v>
       </c>
-      <c r="P4" s="21">
-        <f>(G105+F105+E105)/3</f>
+      <c r="P5" s="21">
+        <f>(G106+F106+E106)/3</f>
         <v>-3.8430459680599771</v>
       </c>
-      <c r="Q4" s="22"/>
-      <c r="R4" s="23"/>
-      <c r="S4" s="23"/>
-      <c r="T4" s="23"/>
-      <c r="U4" s="23"/>
-      <c r="V4" s="23"/>
-      <c r="W4" s="23"/>
-      <c r="X4" s="23"/>
-      <c r="Y4" s="23"/>
-      <c r="Z4" s="23"/>
-      <c r="AA4" s="23"/>
-      <c r="AB4" s="23"/>
-      <c r="AC4" s="23"/>
-      <c r="AD4" s="23"/>
-      <c r="AE4" s="23"/>
-      <c r="AF4" s="23"/>
-      <c r="AG4" s="24"/>
-      <c r="AH4" s="24"/>
-      <c r="AI4" s="25"/>
-      <c r="AJ4" s="25"/>
-      <c r="AK4" s="25"/>
-      <c r="AL4" s="25"/>
-      <c r="AM4" s="24"/>
-      <c r="AN4" s="24"/>
-    </row>
-    <row r="5" spans="1:40" ht="19" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="Q5" s="18"/>
+      <c r="R5" s="16"/>
+      <c r="S5" s="16"/>
+      <c r="T5" s="16"/>
+      <c r="U5" s="16"/>
+      <c r="V5" s="16"/>
+      <c r="W5" s="16"/>
+      <c r="X5" s="16"/>
+      <c r="Y5" s="16"/>
+      <c r="Z5" s="16"/>
+      <c r="AA5" s="16"/>
+      <c r="AB5" s="16"/>
+      <c r="AC5" s="16"/>
+      <c r="AD5" s="16"/>
+      <c r="AE5" s="16"/>
+      <c r="AF5" s="16"/>
+      <c r="AI5" s="22"/>
+      <c r="AJ5" s="22"/>
+      <c r="AK5" s="22"/>
+      <c r="AL5" s="22"/>
+    </row>
+    <row r="6" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B6" s="1">
         <v>647690000</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C6" s="1">
         <v>864032000</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D6" s="1">
         <v>1196313000</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E6" s="1">
         <v>876042000</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F6" s="1">
         <v>1155833000</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G6" s="1">
         <v>1499000000</v>
       </c>
     </row>
-    <row r="6" spans="1:40" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+    <row r="7" spans="1:38" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B7" s="10">
         <v>1914031000</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C7" s="10">
         <v>2787953000</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D7" s="10">
         <v>3608926000</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E7" s="10">
         <v>2502157000</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F7" s="10">
         <v>4835927000</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G7" s="10">
         <v>6900000000</v>
       </c>
-      <c r="M6" s="26" t="s">
+      <c r="M7" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="N6" s="27" t="s">
+      <c r="N7" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="O6" s="27" t="s">
+      <c r="O7" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="P6" s="28" t="s">
+      <c r="P7" s="25" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="7" spans="1:40" ht="19" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+    <row r="8" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B8" s="2">
         <v>0.74719999999999998</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C8" s="2">
         <v>0.76339999999999997</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D8" s="2">
         <v>0.751</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E8" s="2">
         <v>0.74070000000000003</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F8" s="2">
         <v>0.80710000000000004</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G8" s="2">
         <v>0.82150000000000001</v>
       </c>
-      <c r="M7" s="19">
-        <f>G7</f>
+      <c r="M8" s="19">
+        <f>G8</f>
         <v>0.82150000000000001</v>
       </c>
-      <c r="N7" s="20">
-        <f>G21</f>
+      <c r="N8" s="20">
+        <f>G22</f>
         <v>0.24929999999999999</v>
       </c>
-      <c r="O7" s="20">
-        <f>G30</f>
+      <c r="O8" s="20">
+        <f>G31</f>
         <v>0.22539999999999999</v>
       </c>
-      <c r="P7" s="21">
-        <f>G106/G3</f>
+      <c r="P8" s="21">
+        <f>G107/G4</f>
         <v>0.40540540540540543</v>
       </c>
     </row>
-    <row r="8" spans="1:40" ht="19" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+    <row r="9" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B9" s="1">
         <v>400749000</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C9" s="1">
         <v>579193000</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D9" s="1">
         <v>976695000</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E9" s="1">
         <v>2752872000</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F9" s="1">
         <v>1425048000</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G9" s="1">
         <v>1502000000</v>
       </c>
     </row>
-    <row r="9" spans="1:40" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
+    <row r="10" spans="1:38" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="B9" s="18">
-        <f>B8/B3</f>
+      <c r="B10" s="18">
+        <f>B9/B4</f>
         <v>0.15643741063136851</v>
       </c>
-      <c r="C9" s="18">
-        <f t="shared" ref="C9:G9" si="3">C8/C3</f>
+      <c r="C10" s="18">
+        <f t="shared" ref="C10:G10" si="3">C9/C4</f>
         <v>0.15859676313018811</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D10" s="18">
         <f t="shared" si="3"/>
         <v>0.20325627924022094</v>
       </c>
-      <c r="E9" s="18">
+      <c r="E10" s="18">
         <f t="shared" si="3"/>
         <v>0.81489337957888208</v>
       </c>
-      <c r="F9" s="18">
+      <c r="F10" s="18">
         <f t="shared" si="3"/>
         <v>0.23783462622000881</v>
       </c>
-      <c r="G9" s="18">
+      <c r="G10" s="18">
         <f t="shared" si="3"/>
         <v>0.17883081319204666</v>
       </c>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="26" t="s">
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="N9" s="27" t="s">
+      <c r="N10" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="O9" s="27" t="s">
+      <c r="O10" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="P9" s="28" t="s">
+      <c r="P10" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="Q9" s="18"/>
-    </row>
-    <row r="10" spans="1:40" ht="19" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="Q10" s="18"/>
+    </row>
+    <row r="11" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B11" s="1">
         <v>327156000</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C11" s="1">
         <v>479487000</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D11" s="1">
         <v>697181000</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E11" s="1">
         <v>1134851000</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F11" s="1">
         <v>835324000</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G11" s="1">
         <v>950000000</v>
       </c>
-      <c r="M10" s="19">
-        <f>(G9+F9+E9)/3</f>
+      <c r="M11" s="19">
+        <f>(G10+F10+E10)/3</f>
         <v>0.41051960633031248</v>
       </c>
-      <c r="N10" s="20">
-        <f>(G13+F13+E13)/3</f>
+      <c r="N11" s="20">
+        <f>(G14+F14+E14)/3</f>
         <v>0.43828694165068605</v>
       </c>
-      <c r="O10" s="20">
-        <f>(G80+F80+E80)/3</f>
+      <c r="O11" s="20">
+        <f>(G81+F81+E81)/3</f>
         <v>0.38312075768395881</v>
       </c>
-      <c r="P10" s="21">
-        <f>(G89+F89+E89)/3</f>
+      <c r="P11" s="21">
+        <f>(G90+F90+E90)/3</f>
         <v>6.0883618081982701E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:40" ht="19" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+    <row r="12" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B12" s="1">
         <v>871749000</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C12" s="1">
         <v>1101327000</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D12" s="1">
         <v>1621519000</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E12" s="1">
         <v>1175325000</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F12" s="1">
         <v>1186332000</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G12" s="1">
         <v>1516000000</v>
       </c>
     </row>
-    <row r="12" spans="1:40" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+    <row r="13" spans="1:38" ht="23" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B13" s="1">
         <v>1198905000</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C13" s="1">
         <v>1580814000</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D13" s="1">
         <v>2318700000</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E13" s="1">
         <v>2310176000</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F13" s="1">
         <v>2021656000</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G13" s="1">
         <v>2466000000</v>
       </c>
-      <c r="M12" s="26" t="s">
+      <c r="M13" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="N12" s="27" t="s">
+      <c r="N13" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="O12" s="27" t="s">
+      <c r="O13" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="P12" s="28" t="s">
+      <c r="P13" s="25" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="13" spans="1:40" ht="19" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
+    <row r="14" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="B13" s="18">
-        <f>B12/B3</f>
+      <c r="B14" s="18">
+        <f>B13/B4</f>
         <v>0.46800764017627211</v>
       </c>
-      <c r="C13" s="18">
-        <f t="shared" ref="C13:G13" si="4">C12/C3</f>
+      <c r="C14" s="18">
+        <f t="shared" ref="C14:G14" si="4">C13/C4</f>
         <v>0.43286431899364319</v>
       </c>
-      <c r="D13" s="18">
+      <c r="D14" s="18">
         <f t="shared" si="4"/>
         <v>0.48253583224476454</v>
       </c>
-      <c r="E13" s="18">
+      <c r="E14" s="18">
         <f t="shared" si="4"/>
         <v>0.68384840561494453</v>
       </c>
-      <c r="F13" s="18">
+      <c r="F14" s="18">
         <f t="shared" si="4"/>
         <v>0.33740603762500498</v>
       </c>
-      <c r="G13" s="18">
+      <c r="G14" s="18">
         <f t="shared" si="4"/>
         <v>0.29360638171210857</v>
       </c>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="18"/>
-      <c r="L13" s="18"/>
-      <c r="M13" s="29">
-        <f>G28/G72</f>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="26">
+        <f>G29/G73</f>
         <v>0.34046762589928059</v>
       </c>
-      <c r="N13" s="30">
-        <f>G28/G54</f>
+      <c r="N14" s="27">
+        <f>G29/G55</f>
         <v>0.11803217358772915</v>
       </c>
-      <c r="O13" s="30">
-        <f>(G28-G98)/G73</f>
+      <c r="O14" s="27">
+        <f>(G29-G99)/G74</f>
         <v>0.11803217358772915</v>
       </c>
-      <c r="P13" s="31">
-        <f>(G61+G56)/G72</f>
+      <c r="P14" s="28">
+        <f>(G62+G57)/G73</f>
         <v>0.42104316546762588</v>
       </c>
-      <c r="Q13" s="18"/>
-    </row>
-    <row r="14" spans="1:40" ht="19" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="Q14" s="18"/>
+    </row>
+    <row r="15" spans="1:38" ht="19" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B15" s="1">
         <v>395739000</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C15" s="1">
         <v>609202000</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D15" s="1">
         <v>815074000</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E15" s="1">
         <v>877901000</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F15" s="1">
         <v>847057000</v>
       </c>
-      <c r="G14" s="1">
+      <c r="G15" s="1">
         <v>1041000000</v>
       </c>
     </row>
-    <row r="15" spans="1:40" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+    <row r="16" spans="1:38" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B16" s="1">
         <v>1995393000</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C16" s="1">
         <v>2769209000</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D16" s="1">
         <v>4110469000</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E16" s="1">
         <v>5940949000</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F16" s="1">
         <v>4293761000</v>
       </c>
-      <c r="G15" s="1">
+      <c r="G16" s="1">
         <v>5009000000</v>
       </c>
-      <c r="M15" s="26" t="s">
+      <c r="M16" s="23" t="s">
         <v>122</v>
-      </c>
-    </row>
-    <row r="16" spans="1:40" ht="19" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="1">
-        <v>2643083000</v>
-      </c>
-      <c r="C16" s="1">
-        <v>3633241000</v>
-      </c>
-      <c r="D16" s="1">
-        <v>5306782000</v>
-      </c>
-      <c r="E16" s="1">
-        <v>6816991000</v>
-      </c>
-      <c r="F16" s="1">
-        <v>5449594000</v>
-      </c>
-      <c r="G16" s="1">
-        <v>6508000000</v>
-      </c>
-      <c r="M16" s="19">
-        <f>(SUM(C35:G35)/5)</f>
-        <v>0.14224609231543348</v>
       </c>
     </row>
     <row r="17" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="1">
+        <v>2643083000</v>
+      </c>
+      <c r="C17" s="1">
+        <v>3633241000</v>
+      </c>
+      <c r="D17" s="1">
+        <v>5306782000</v>
+      </c>
+      <c r="E17" s="1">
+        <v>6816991000</v>
+      </c>
+      <c r="F17" s="1">
+        <v>5449594000</v>
+      </c>
+      <c r="G17" s="1">
+        <v>6508000000</v>
+      </c>
+      <c r="M17" s="19">
+        <f>(SUM(C36:G36)/5)</f>
+        <v>0.14224609231543348</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B18" s="1">
         <v>16403000</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C18" s="1">
         <v>26143000</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D18" s="1">
         <v>9968000</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E18" s="1">
         <v>171688000</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F18" s="1">
         <v>437599000</v>
       </c>
-      <c r="G17" s="1">
+      <c r="G18" s="1">
         <v>24000000</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="21" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+    <row r="19" spans="1:17" ht="21" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B19" s="1">
         <v>79342000</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C19" s="1">
         <v>82401000</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D19" s="1">
         <v>114162000</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E19" s="1">
         <v>125876000</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F19" s="1">
         <v>138319000</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G19" s="1">
         <v>81000000</v>
       </c>
-      <c r="M18" s="37" t="s">
+      <c r="M19" s="66" t="s">
         <v>157</v>
       </c>
-      <c r="N18" s="38"/>
-    </row>
-    <row r="19" spans="1:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="N19" s="67"/>
+    </row>
+    <row r="20" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="10">
+      <c r="B20" s="10">
         <v>36646000</v>
       </c>
-      <c r="C19" s="10">
+      <c r="C20" s="10">
         <v>155577000</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D20" s="10">
         <v>-287573000</v>
       </c>
-      <c r="E19" s="10">
+      <c r="E20" s="10">
         <v>-4384374000</v>
       </c>
-      <c r="F19" s="10">
+      <c r="F20" s="10">
         <v>275711000</v>
       </c>
-      <c r="G19" s="10">
+      <c r="G20" s="10">
         <v>2094000000</v>
       </c>
-      <c r="M19" s="39" t="s">
+      <c r="M20" s="68" t="s">
         <v>124</v>
       </c>
-      <c r="N19" s="40"/>
-    </row>
-    <row r="20" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="17" t="s">
+      <c r="N20" s="69"/>
+    </row>
+    <row r="21" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="18">
-        <f>(C19/B19)-1</f>
+      <c r="B21" s="1"/>
+      <c r="C21" s="18">
+        <f>(C20/B20)-1</f>
         <v>3.2454019538285213</v>
       </c>
-      <c r="D20" s="18">
-        <f>(D19/C19)-1</f>
+      <c r="D21" s="18">
+        <f>(D20/C20)-1</f>
         <v>-2.8484287523220013</v>
       </c>
-      <c r="E20" s="18">
-        <f>(E19/D19)-1</f>
+      <c r="E21" s="18">
+        <f>(E20/D20)-1</f>
         <v>14.24612533165492</v>
       </c>
-      <c r="F20" s="18">
-        <f t="shared" ref="F20:G20" si="5">(F19/E19)-1</f>
+      <c r="F21" s="18">
+        <f t="shared" ref="F21:G21" si="5">(F20/E20)-1</f>
         <v>-1.0628849181205799</v>
       </c>
-      <c r="G20" s="18">
+      <c r="G21" s="18">
         <f t="shared" si="5"/>
         <v>6.5949091621299116</v>
       </c>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
-      <c r="K20" s="18"/>
-      <c r="L20" s="18"/>
-      <c r="M20" s="32" t="s">
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18"/>
+      <c r="M21" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="N20" s="33">
-        <f>G17</f>
+      <c r="N21" s="30">
+        <f>G18</f>
         <v>24000000</v>
       </c>
-      <c r="O20" s="18"/>
-      <c r="P20" s="18"/>
-      <c r="Q20" s="18"/>
-    </row>
-    <row r="21" spans="1:17" ht="20" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+      <c r="O21" s="18"/>
+      <c r="P21" s="18"/>
+      <c r="Q21" s="18"/>
+    </row>
+    <row r="22" spans="1:17" ht="20" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B22" s="2">
         <v>1.43E-2</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C22" s="2">
         <v>4.2599999999999999E-2</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D22" s="2">
         <v>-5.9799999999999999E-2</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E22" s="2">
         <v>-1.2978000000000001</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F22" s="2">
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="G21" s="2">
+      <c r="G22" s="2">
         <v>0.24929999999999999</v>
       </c>
-      <c r="M21" s="32" t="s">
+      <c r="M22" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="N21" s="33">
-        <f>G56</f>
+      <c r="N22" s="30">
+        <f>G57</f>
         <v>59000000</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="20" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+    <row r="23" spans="1:17" ht="20" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="10">
+      <c r="B23" s="10">
         <v>-81362000</v>
       </c>
-      <c r="C22" s="10">
+      <c r="C23" s="10">
         <v>18744000</v>
       </c>
-      <c r="D22" s="10">
+      <c r="D23" s="10">
         <v>-501543000</v>
       </c>
-      <c r="E22" s="10">
+      <c r="E23" s="10">
         <v>-3590147000</v>
       </c>
-      <c r="F22" s="10">
+      <c r="F23" s="10">
         <v>429317000</v>
       </c>
-      <c r="G22" s="10">
+      <c r="G23" s="10">
         <v>1891000000</v>
       </c>
-      <c r="M22" s="32" t="s">
+      <c r="M23" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="N22" s="33">
-        <f>G61</f>
+      <c r="N23" s="30">
+        <f>G62</f>
         <v>2282000000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" ht="20" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B23" s="2">
-        <v>-3.1800000000000002E-2</v>
-      </c>
-      <c r="C23" s="2">
-        <v>5.1000000000000004E-3</v>
-      </c>
-      <c r="D23" s="2">
-        <v>-0.10440000000000001</v>
-      </c>
-      <c r="E23" s="2">
-        <v>-1.0627</v>
-      </c>
-      <c r="F23" s="2">
-        <v>7.17E-2</v>
-      </c>
-      <c r="G23" s="2">
-        <v>0.22509999999999999</v>
-      </c>
-      <c r="M23" s="41" t="s">
-        <v>127</v>
-      </c>
-      <c r="N23" s="42">
-        <f>N20/(N21+N22)</f>
-        <v>1.0252029047415635E-2</v>
       </c>
     </row>
     <row r="24" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="2">
+        <v>-3.1800000000000002E-2</v>
+      </c>
+      <c r="C24" s="2">
+        <v>5.1000000000000004E-3</v>
+      </c>
+      <c r="D24" s="2">
+        <v>-0.10440000000000001</v>
+      </c>
+      <c r="E24" s="2">
+        <v>-1.0627</v>
+      </c>
+      <c r="F24" s="2">
+        <v>7.17E-2</v>
+      </c>
+      <c r="G24" s="2">
+        <v>0.22509999999999999</v>
+      </c>
+      <c r="M24" s="34" t="s">
+        <v>127</v>
+      </c>
+      <c r="N24" s="35">
+        <f>N21/(N22+N23)</f>
+        <v>1.0252029047415635E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" ht="20" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B25" s="1">
         <v>22263000</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C25" s="1">
         <v>28289000</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D25" s="1">
         <v>89840000</v>
       </c>
-      <c r="E24" s="1">
+      <c r="E25" s="1">
         <v>-1091791000</v>
       </c>
-      <c r="F24" s="1">
+      <c r="F25" s="1">
         <v>-729524000</v>
       </c>
-      <c r="G24" s="1">
+      <c r="G25" s="1">
         <v>98000000</v>
       </c>
-      <c r="M24" s="32" t="s">
+      <c r="M25" s="29" t="s">
         <v>128</v>
       </c>
-      <c r="N24" s="33">
-        <f>G27</f>
+      <c r="N25" s="30">
+        <f>G28</f>
         <v>96000000</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="20" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
+    <row r="26" spans="1:17" ht="20" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="10">
+      <c r="B26" s="10">
         <v>-59099000</v>
       </c>
-      <c r="C25" s="10">
+      <c r="C26" s="10">
         <v>47033000</v>
       </c>
-      <c r="D25" s="10">
+      <c r="D26" s="10">
         <v>-411703000</v>
       </c>
-      <c r="E25" s="10">
+      <c r="E26" s="10">
         <v>-4681938000</v>
       </c>
-      <c r="F25" s="10">
+      <c r="F26" s="10">
         <v>-300207000</v>
       </c>
-      <c r="G25" s="10">
+      <c r="G26" s="10">
         <v>1989000000</v>
       </c>
-      <c r="M25" s="32" t="s">
+      <c r="M26" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="N25" s="33">
-        <f>G25</f>
+      <c r="N26" s="30">
+        <f>G26</f>
         <v>1989000000</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" ht="20" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B26" s="2">
-        <v>-2.3099999999999999E-2</v>
-      </c>
-      <c r="C26" s="2">
-        <v>1.29E-2</v>
-      </c>
-      <c r="D26" s="2">
-        <v>-8.5699999999999998E-2</v>
-      </c>
-      <c r="E26" s="2">
-        <v>-1.3858999999999999</v>
-      </c>
-      <c r="F26" s="2">
-        <v>-5.0099999999999999E-2</v>
-      </c>
-      <c r="G26" s="2">
-        <v>0.23680000000000001</v>
-      </c>
-      <c r="M26" s="41" t="s">
-        <v>129</v>
-      </c>
-      <c r="N26" s="42">
-        <f>N24/N25</f>
-        <v>4.8265460030165915E-2</v>
       </c>
     </row>
     <row r="27" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" s="2">
+        <v>-2.3099999999999999E-2</v>
+      </c>
+      <c r="C27" s="2">
+        <v>1.29E-2</v>
+      </c>
+      <c r="D27" s="2">
+        <v>-8.5699999999999998E-2</v>
+      </c>
+      <c r="E27" s="2">
+        <v>-1.3858999999999999</v>
+      </c>
+      <c r="F27" s="2">
+        <v>-5.0099999999999999E-2</v>
+      </c>
+      <c r="G27" s="2">
+        <v>0.23680000000000001</v>
+      </c>
+      <c r="M27" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="N27" s="35">
+        <f>N25/N26</f>
+        <v>4.8265460030165915E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" ht="20" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B28" s="1">
         <v>10947000</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C28" s="1">
         <v>63893000</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D28" s="1">
         <v>262636000</v>
       </c>
-      <c r="E27" s="1">
+      <c r="E28" s="1">
         <v>-97222000</v>
       </c>
-      <c r="F27" s="1">
+      <c r="F28" s="1">
         <v>51827000</v>
       </c>
-      <c r="G27" s="1">
+      <c r="G28" s="1">
         <v>96000000</v>
       </c>
-      <c r="M27" s="43" t="s">
+      <c r="M28" s="36" t="s">
         <v>130</v>
       </c>
-      <c r="N27" s="44">
-        <f>N23*(1-N26)</f>
+      <c r="N28" s="37">
+        <f>N24*(1-N27)</f>
         <v>9.7572101491994953E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:17" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="7" t="s">
+    <row r="29" spans="1:17" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B28" s="11">
+      <c r="B29" s="11">
         <v>-70046000</v>
       </c>
-      <c r="C28" s="11">
+      <c r="C29" s="11">
         <v>-16860000</v>
       </c>
-      <c r="D28" s="11">
+      <c r="D29" s="11">
         <v>-674339000</v>
       </c>
-      <c r="E28" s="11">
+      <c r="E29" s="11">
         <v>-4584716000</v>
       </c>
-      <c r="F28" s="11">
+      <c r="F29" s="11">
         <v>-352034000</v>
       </c>
-      <c r="G28" s="11">
+      <c r="G29" s="11">
         <v>1893000000</v>
       </c>
-      <c r="M28" s="39" t="s">
+      <c r="M29" s="68" t="s">
         <v>131</v>
       </c>
-      <c r="N28" s="40"/>
-    </row>
-    <row r="29" spans="1:17" ht="20" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="17" t="s">
+      <c r="N29" s="69"/>
+    </row>
+    <row r="30" spans="1:17" ht="20" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="B29" s="1"/>
-      <c r="C29" s="18">
-        <f>(C28/B28)-1</f>
+      <c r="B30" s="1"/>
+      <c r="C30" s="18">
+        <f>(C29/B29)-1</f>
         <v>-0.75930103075122068</v>
       </c>
-      <c r="D29" s="18">
-        <f>(D28/C28)-1</f>
+      <c r="D30" s="18">
+        <f>(D29/C29)-1</f>
         <v>38.996381969157767</v>
       </c>
-      <c r="E29" s="18">
-        <f>(E28/D28)-1</f>
+      <c r="E30" s="18">
+        <f>(E29/D29)-1</f>
         <v>5.7988296687571088</v>
       </c>
-      <c r="F29" s="18">
-        <f t="shared" ref="F29:G29" si="6">(F28/E28)-1</f>
+      <c r="F30" s="18">
+        <f t="shared" ref="F30:G30" si="6">(F29/E29)-1</f>
         <v>-0.92321574553363828</v>
       </c>
-      <c r="G29" s="18">
+      <c r="G30" s="18">
         <f t="shared" si="6"/>
         <v>-6.377321508717908</v>
       </c>
-      <c r="H29" s="18"/>
-      <c r="I29" s="18"/>
-      <c r="J29" s="18"/>
-      <c r="K29" s="18"/>
-      <c r="L29" s="18"/>
-      <c r="M29" s="32" t="s">
+      <c r="H30" s="18"/>
+      <c r="I30" s="18"/>
+      <c r="J30" s="18"/>
+      <c r="K30" s="18"/>
+      <c r="L30" s="18"/>
+      <c r="M30" s="29" t="s">
         <v>105</v>
       </c>
-      <c r="N29" s="34">
+      <c r="N30" s="31">
         <v>4.095E-2</v>
       </c>
-      <c r="O29" s="18"/>
-      <c r="P29" s="18"/>
-      <c r="Q29" s="18"/>
-    </row>
-    <row r="30" spans="1:17" ht="20" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B30" s="2">
-        <v>-2.7300000000000001E-2</v>
-      </c>
-      <c r="C30" s="2">
-        <v>-4.5999999999999999E-3</v>
-      </c>
-      <c r="D30" s="2">
-        <v>-0.14030000000000001</v>
-      </c>
-      <c r="E30" s="2">
-        <v>-1.3571</v>
-      </c>
-      <c r="F30" s="2">
-        <v>-5.8799999999999998E-2</v>
-      </c>
-      <c r="G30" s="2">
-        <v>0.22539999999999999</v>
-      </c>
-      <c r="M30" s="32" t="s">
-        <v>132</v>
-      </c>
-      <c r="N30" s="45">
-        <v>1.22</v>
-      </c>
+      <c r="O30" s="18"/>
+      <c r="P30" s="18"/>
+      <c r="Q30" s="18"/>
     </row>
     <row r="31" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B31" s="12">
-        <v>-0.13</v>
-      </c>
-      <c r="C31" s="12">
-        <v>-0.03</v>
-      </c>
-      <c r="D31" s="12">
-        <v>-1.29</v>
-      </c>
-      <c r="E31" s="12">
-        <v>-16.12</v>
-      </c>
-      <c r="F31" s="12">
-        <v>-0.56999999999999995</v>
-      </c>
-      <c r="G31" s="12">
-        <v>3.07</v>
-      </c>
-      <c r="M31" s="32" t="s">
-        <v>133</v>
-      </c>
-      <c r="N31" s="34">
-        <v>8.4000000000000005E-2</v>
+        <v>23</v>
+      </c>
+      <c r="B31" s="2">
+        <v>-2.7300000000000001E-2</v>
+      </c>
+      <c r="C31" s="2">
+        <v>-4.5999999999999999E-3</v>
+      </c>
+      <c r="D31" s="2">
+        <v>-0.14030000000000001</v>
+      </c>
+      <c r="E31" s="2">
+        <v>-1.3571</v>
+      </c>
+      <c r="F31" s="2">
+        <v>-5.8799999999999998E-2</v>
+      </c>
+      <c r="G31" s="2">
+        <v>0.22539999999999999</v>
+      </c>
+      <c r="M31" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="N31" s="38">
+        <v>1.22</v>
       </c>
     </row>
     <row r="32" spans="1:17" ht="20" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B32" s="12">
         <v>-0.13</v>
@@ -3663,44 +3481,46 @@
       <c r="G32" s="12">
         <v>3.07</v>
       </c>
-      <c r="M32" s="43" t="s">
+      <c r="M32" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="N32" s="31">
+        <v>8.4000000000000005E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" ht="20" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B33" s="12">
+        <v>-0.13</v>
+      </c>
+      <c r="C33" s="12">
+        <v>-0.03</v>
+      </c>
+      <c r="D33" s="12">
+        <v>-1.29</v>
+      </c>
+      <c r="E33" s="12">
+        <v>-16.12</v>
+      </c>
+      <c r="F33" s="12">
+        <v>-0.56999999999999995</v>
+      </c>
+      <c r="G33" s="12">
+        <v>3.07</v>
+      </c>
+      <c r="M33" s="36" t="s">
         <v>134</v>
       </c>
-      <c r="N32" s="44">
-        <f>(N29)+((N30)*(N31-N29))</f>
+      <c r="N33" s="37">
+        <f>(N30)+((N31)*(N32-N30))</f>
         <v>9.3470999999999999E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
+    <row r="34" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="B33" s="1">
-        <v>521709000</v>
-      </c>
-      <c r="C33" s="1">
-        <v>530945000</v>
-      </c>
-      <c r="D33" s="1">
-        <v>521709000</v>
-      </c>
-      <c r="E33" s="1">
-        <v>284363000</v>
-      </c>
-      <c r="F33" s="1">
-        <v>615891000</v>
-      </c>
-      <c r="G33" s="1">
-        <v>615891000</v>
-      </c>
-      <c r="M33" s="39" t="s">
-        <v>135</v>
-      </c>
-      <c r="N33" s="40"/>
-    </row>
-    <row r="34" spans="1:14" ht="20" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
-        <v>27</v>
       </c>
       <c r="B34" s="1">
         <v>521709000</v>
@@ -3720,403 +3540,407 @@
       <c r="G34" s="1">
         <v>615891000</v>
       </c>
-      <c r="M34" s="32" t="s">
+      <c r="M34" s="68" t="s">
+        <v>135</v>
+      </c>
+      <c r="N34" s="69"/>
+    </row>
+    <row r="35" spans="1:14" ht="20" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B35" s="1">
+        <v>521709000</v>
+      </c>
+      <c r="C35" s="1">
+        <v>530945000</v>
+      </c>
+      <c r="D35" s="1">
+        <v>521709000</v>
+      </c>
+      <c r="E35" s="1">
+        <v>284363000</v>
+      </c>
+      <c r="F35" s="1">
+        <v>615891000</v>
+      </c>
+      <c r="G35" s="1">
+        <v>615891000</v>
+      </c>
+      <c r="M35" s="29" t="s">
         <v>136</v>
       </c>
-      <c r="N34" s="33">
-        <f>N21+N22</f>
+      <c r="N35" s="30">
+        <f>N22+N23</f>
         <v>2341000000</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="20" x14ac:dyDescent="0.25">
-      <c r="A35" s="17" t="s">
+    <row r="36" spans="1:14" ht="20" x14ac:dyDescent="0.25">
+      <c r="A36" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="B35" s="1"/>
-      <c r="C35" s="36">
-        <f>(C34-B34)/B34</f>
+      <c r="B36" s="1"/>
+      <c r="C36" s="33">
+        <f>(C35-B35)/B35</f>
         <v>1.7703355702125129E-2</v>
       </c>
-      <c r="D35" s="36">
-        <f t="shared" ref="D35:G35" si="7">(D34-C34)/C34</f>
+      <c r="D36" s="33">
+        <f t="shared" ref="D36:G36" si="7">(D35-C35)/C35</f>
         <v>-1.7395398770117431E-2</v>
       </c>
-      <c r="E35" s="36">
+      <c r="E36" s="33">
         <f t="shared" si="7"/>
         <v>-0.45493943941929316</v>
       </c>
-      <c r="F35" s="36">
+      <c r="F36" s="33">
         <f t="shared" si="7"/>
         <v>1.1658619440644529</v>
       </c>
-      <c r="G35" s="36">
+      <c r="G36" s="33">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="M35" s="41" t="s">
+      <c r="M36" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="N35" s="42">
-        <f>N34/N38</f>
+      <c r="N36" s="35">
+        <f>N35/N39</f>
         <v>2.8430551001323762E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="20" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
+    <row r="37" spans="1:14" ht="20" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B36" s="13" t="s">
+      <c r="B37" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="C36" s="13" t="s">
+      <c r="C37" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="D36" s="13" t="s">
+      <c r="D37" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="E36" s="13" t="s">
+      <c r="E37" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="F36" s="13" t="s">
+      <c r="F37" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="G36" s="13" t="s">
+      <c r="G37" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="M36" s="32" t="s">
+      <c r="M37" s="29" t="s">
         <v>138</v>
       </c>
-      <c r="N36" s="46">
+      <c r="N37" s="39">
         <v>80000000000</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
+    <row r="38" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B37" s="9" t="s">
+      <c r="B38" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="C37" s="9" t="s">
+      <c r="C38" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="D37" s="9" t="s">
+      <c r="D38" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="E37" s="9" t="s">
+      <c r="E38" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="F37" s="9" t="s">
+      <c r="F38" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="G37" s="9" t="s">
+      <c r="G38" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="M37" s="41" t="s">
+      <c r="M38" s="34" t="s">
         <v>139</v>
       </c>
-      <c r="N37" s="42">
-        <f>N36/N38</f>
+      <c r="N38" s="35">
+        <f>N37/N39</f>
         <v>0.97156944899867625</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="20" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
+    <row r="39" spans="1:14" ht="20" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C38" s="1">
+      <c r="B39" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C39" s="1">
         <v>2140877000</v>
       </c>
-      <c r="D38" s="1">
+      <c r="D39" s="1">
         <v>2013547000</v>
       </c>
-      <c r="E38" s="1">
+      <c r="E39" s="1">
         <v>5480557000</v>
       </c>
-      <c r="F38" s="1">
+      <c r="F39" s="1">
         <v>6067438000</v>
       </c>
-      <c r="G38" s="1">
+      <c r="G39" s="1">
         <v>7378000000</v>
       </c>
-      <c r="M38" s="43" t="s">
+      <c r="M39" s="36" t="s">
         <v>140</v>
       </c>
-      <c r="N38" s="47">
-        <f>N34+N36</f>
+      <c r="N39" s="40">
+        <f>N35+N37</f>
         <v>82341000000</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
+    <row r="40" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C39" s="1">
+      <c r="B40" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C40" s="1">
         <v>1188431000</v>
       </c>
-      <c r="D39" s="1">
+      <c r="D40" s="1">
         <v>1060726000</v>
       </c>
-      <c r="E39" s="1">
+      <c r="E40" s="1">
         <v>910700000</v>
       </c>
-      <c r="F39" s="1">
+      <c r="F40" s="1">
         <v>2255038000</v>
       </c>
-      <c r="G39" s="1">
+      <c r="G40" s="1">
         <v>2244000000</v>
       </c>
-      <c r="M39" s="39" t="s">
+      <c r="M40" s="68" t="s">
         <v>141</v>
       </c>
-      <c r="N39" s="40"/>
-    </row>
-    <row r="40" spans="1:14" ht="20" x14ac:dyDescent="0.25">
-      <c r="A40" s="5" t="s">
+      <c r="N40" s="69"/>
+    </row>
+    <row r="41" spans="1:14" ht="20" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C40" s="1">
+      <c r="B41" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C41" s="1">
         <v>3329308000</v>
       </c>
-      <c r="D40" s="1">
+      <c r="D41" s="1">
         <v>3074273000</v>
       </c>
-      <c r="E40" s="1">
+      <c r="E41" s="1">
         <v>6391257000</v>
       </c>
-      <c r="F40" s="1">
+      <c r="F41" s="1">
         <v>8322476000</v>
       </c>
-      <c r="G40" s="1">
+      <c r="G41" s="1">
         <v>9622000000</v>
       </c>
-      <c r="M40" s="48" t="s">
+      <c r="M41" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="N40" s="49">
-        <f>(N35*N27)+(N37*N32)</f>
+      <c r="N41" s="42">
+        <f>(N36*N28)+(N38*N33)</f>
         <v>9.1090970828132709E-2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C41" s="1">
-        <v>2305011000</v>
-      </c>
-      <c r="D41" s="1">
-        <v>3145457000</v>
-      </c>
-      <c r="E41" s="1">
-        <v>2181329000</v>
-      </c>
-      <c r="F41" s="1">
-        <v>3715471000</v>
-      </c>
-      <c r="G41" s="1">
-        <v>4783000000</v>
       </c>
     </row>
     <row r="42" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>93</v>
+      <c r="C42" s="1">
+        <v>2305011000</v>
+      </c>
+      <c r="D42" s="1">
+        <v>3145457000</v>
+      </c>
+      <c r="E42" s="1">
+        <v>2181329000</v>
+      </c>
+      <c r="F42" s="1">
+        <v>3715471000</v>
+      </c>
+      <c r="G42" s="1">
+        <v>4783000000</v>
       </c>
     </row>
     <row r="43" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C43" s="1">
+      <c r="B44" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C44" s="1">
         <v>240213000</v>
       </c>
-      <c r="D43" s="1">
+      <c r="D44" s="1">
         <v>341713000</v>
       </c>
-      <c r="E43" s="1">
+      <c r="E44" s="1">
         <v>343800000</v>
       </c>
-      <c r="F43" s="1">
+      <c r="F44" s="1">
         <v>348433000</v>
       </c>
-      <c r="G43" s="1">
+      <c r="G44" s="1">
         <v>456000000</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="A44" s="6" t="s">
+    <row r="45" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B44" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="C44" s="10">
+      <c r="B45" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="C45" s="10">
         <v>5874532000</v>
       </c>
-      <c r="D44" s="10">
+      <c r="D45" s="10">
         <v>6561443000</v>
       </c>
-      <c r="E44" s="10">
+      <c r="E45" s="10">
         <v>8916386000</v>
       </c>
-      <c r="F44" s="10">
+      <c r="F45" s="10">
         <v>12386380000</v>
       </c>
-      <c r="G44" s="10">
+      <c r="G45" s="10">
         <v>14861000000</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C45" s="1">
-        <v>309408000</v>
-      </c>
-      <c r="D45" s="1">
-        <v>686867000</v>
-      </c>
-      <c r="E45" s="1">
-        <v>654262000</v>
-      </c>
-      <c r="F45" s="1">
-        <v>428621000</v>
-      </c>
-      <c r="G45" s="1">
-        <v>259000000</v>
       </c>
     </row>
     <row r="46" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>93</v>
       </c>
       <c r="C46" s="1">
-        <v>289861000</v>
+        <v>309408000</v>
       </c>
       <c r="D46" s="1">
-        <v>652088000</v>
+        <v>686867000</v>
       </c>
       <c r="E46" s="1">
-        <v>655801000</v>
+        <v>654262000</v>
       </c>
       <c r="F46" s="1">
-        <v>652602000</v>
+        <v>428621000</v>
       </c>
       <c r="G46" s="1">
-        <v>650000000</v>
+        <v>259000000</v>
       </c>
     </row>
     <row r="47" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>93</v>
       </c>
       <c r="C47" s="1">
-        <v>28756000</v>
+        <v>289861000</v>
       </c>
       <c r="D47" s="1">
-        <v>102912000</v>
+        <v>652088000</v>
       </c>
       <c r="E47" s="1">
-        <v>75886000</v>
+        <v>655801000</v>
       </c>
       <c r="F47" s="1">
-        <v>52308000</v>
+        <v>652602000</v>
       </c>
       <c r="G47" s="1">
-        <v>34000000</v>
+        <v>650000000</v>
       </c>
     </row>
     <row r="48" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>93</v>
       </c>
       <c r="C48" s="1">
-        <v>318617000</v>
+        <v>28756000</v>
       </c>
       <c r="D48" s="1">
-        <v>755000000</v>
+        <v>102912000</v>
       </c>
       <c r="E48" s="1">
-        <v>731687000</v>
+        <v>75886000</v>
       </c>
       <c r="F48" s="1">
-        <v>704910000</v>
+        <v>52308000</v>
       </c>
       <c r="G48" s="1">
-        <v>684000000</v>
+        <v>34000000</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C49" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>93</v>
+      <c r="C49" s="1">
+        <v>318617000</v>
+      </c>
+      <c r="D49" s="1">
+        <v>755000000</v>
+      </c>
+      <c r="E49" s="1">
+        <v>731687000</v>
+      </c>
+      <c r="F49" s="1">
+        <v>704910000</v>
+      </c>
+      <c r="G49" s="1">
+        <v>684000000</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>93</v>
@@ -4139,260 +3963,260 @@
     </row>
     <row r="51" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C51" s="1">
-        <v>110532000</v>
-      </c>
-      <c r="D51" s="1">
-        <v>306809000</v>
-      </c>
-      <c r="E51" s="1">
-        <v>189164000</v>
-      </c>
-      <c r="F51" s="1">
-        <v>188563000</v>
-      </c>
-      <c r="G51" s="1">
-        <v>234000000</v>
+      <c r="C51" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>93</v>
       </c>
       <c r="C52" s="1">
-        <v>738557000</v>
+        <v>110532000</v>
       </c>
       <c r="D52" s="1">
-        <v>1748676000</v>
+        <v>306809000</v>
       </c>
       <c r="E52" s="1">
-        <v>1575113000</v>
+        <v>189164000</v>
       </c>
       <c r="F52" s="1">
-        <v>1322094000</v>
+        <v>188563000</v>
       </c>
       <c r="G52" s="1">
-        <v>1177000000</v>
+        <v>234000000</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C53" s="1">
+        <v>738557000</v>
+      </c>
+      <c r="D53" s="1">
+        <v>1748676000</v>
+      </c>
+      <c r="E53" s="1">
+        <v>1575113000</v>
+      </c>
+      <c r="F53" s="1">
+        <v>1322094000</v>
+      </c>
+      <c r="G53" s="1">
+        <v>1177000000</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A54" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B53" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A54" s="7" t="s">
+      <c r="B54" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A55" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B54" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="C54" s="11">
+      <c r="B55" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="C55" s="11">
         <v>6613089000</v>
       </c>
-      <c r="D54" s="11">
+      <c r="D55" s="11">
         <v>8310119000</v>
       </c>
-      <c r="E54" s="11">
+      <c r="E55" s="11">
         <v>10491499000</v>
       </c>
-      <c r="F54" s="11">
+      <c r="F55" s="11">
         <v>13708474000</v>
       </c>
-      <c r="G54" s="11">
+      <c r="G55" s="11">
         <v>16038000000</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A55" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C55" s="1">
-        <v>70630000</v>
-      </c>
-      <c r="D55" s="1">
-        <v>151417000</v>
-      </c>
-      <c r="E55" s="1">
-        <v>79898000</v>
-      </c>
-      <c r="F55" s="1">
-        <v>118361000</v>
-      </c>
-      <c r="G55" s="1">
-        <v>137000000</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>93</v>
+      <c r="C56" s="1">
+        <v>70630000</v>
       </c>
       <c r="D56" s="1">
-        <v>38022000</v>
+        <v>151417000</v>
       </c>
       <c r="E56" s="1">
-        <v>83341000</v>
+        <v>79898000</v>
       </c>
       <c r="F56" s="1">
-        <v>63479000</v>
+        <v>118361000</v>
       </c>
       <c r="G56" s="1">
-        <v>59000000</v>
+        <v>137000000</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C57" s="1">
-        <v>159901000</v>
+      <c r="C57" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="D57" s="1">
-        <v>207462000</v>
+        <v>38022000</v>
       </c>
       <c r="E57" s="1">
-        <v>165257000</v>
+        <v>83341000</v>
       </c>
       <c r="F57" s="1">
-        <v>334728000</v>
-      </c>
-      <c r="G57" s="1" t="s">
-        <v>93</v>
+        <v>63479000</v>
+      </c>
+      <c r="G57" s="1">
+        <v>59000000</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C58" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="G58" s="1">
-        <v>1182000000</v>
+      <c r="C58" s="1">
+        <v>159901000</v>
+      </c>
+      <c r="D58" s="1">
+        <v>207462000</v>
+      </c>
+      <c r="E58" s="1">
+        <v>165257000</v>
+      </c>
+      <c r="F58" s="1">
+        <v>334728000</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G59" s="1">
+        <v>1182000000</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A60" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B59" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C59" s="1">
+      <c r="B60" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C60" s="1">
         <v>3505479000</v>
       </c>
-      <c r="D59" s="1">
+      <c r="D60" s="1">
         <v>4836863000</v>
       </c>
-      <c r="E59" s="1">
+      <c r="E60" s="1">
         <v>4811283000</v>
       </c>
-      <c r="F59" s="1">
+      <c r="F60" s="1">
         <v>5842714000</v>
       </c>
-      <c r="G59" s="1">
+      <c r="G60" s="1">
         <v>6600000000</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A60" s="6" t="s">
+    <row r="61" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A61" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B60" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="C60" s="10">
+      <c r="B61" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="C61" s="10">
         <v>3736010000</v>
       </c>
-      <c r="D60" s="10">
+      <c r="D61" s="10">
         <v>5233764000</v>
       </c>
-      <c r="E60" s="10">
+      <c r="E61" s="10">
         <v>5139779000</v>
       </c>
-      <c r="F60" s="10">
+      <c r="F61" s="10">
         <v>6359282000</v>
       </c>
-      <c r="G60" s="10">
+      <c r="G61" s="10">
         <v>7978000000</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A61" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D61" s="1">
-        <v>381374000</v>
-      </c>
-      <c r="E61" s="1">
-        <v>2246467000</v>
-      </c>
-      <c r="F61" s="1">
-        <v>2355020000</v>
-      </c>
-      <c r="G61" s="1">
-        <v>2282000000</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>93</v>
@@ -4400,22 +4224,22 @@
       <c r="C62" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D62" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F62" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="G62" s="1" t="s">
-        <v>93</v>
+      <c r="D62" s="1">
+        <v>381374000</v>
+      </c>
+      <c r="E62" s="1">
+        <v>2246467000</v>
+      </c>
+      <c r="F62" s="1">
+        <v>2355020000</v>
+      </c>
+      <c r="G62" s="1">
+        <v>2282000000</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>93</v>
@@ -4438,30 +4262,30 @@
     </row>
     <row r="64" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+      <c r="A65" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C64" s="1">
-        <v>3394387000</v>
-      </c>
-      <c r="D64" s="1">
-        <v>3502666000</v>
-      </c>
-      <c r="E64" s="1">
-        <v>203470000</v>
-      </c>
-      <c r="F64" s="1">
-        <v>218459000</v>
-      </c>
-      <c r="G64" s="1">
-        <v>218000000</v>
-      </c>
-    </row>
-    <row r="65" spans="1:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="A65" s="5" t="s">
-        <v>56</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>93</v>
@@ -4470,429 +4294,429 @@
         <v>3394387000</v>
       </c>
       <c r="D65" s="1">
+        <v>3502666000</v>
+      </c>
+      <c r="E65" s="1">
+        <v>203470000</v>
+      </c>
+      <c r="F65" s="1">
+        <v>218459000</v>
+      </c>
+      <c r="G65" s="1">
+        <v>218000000</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+      <c r="A66" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C66" s="1">
+        <v>3394387000</v>
+      </c>
+      <c r="D66" s="1">
         <v>3884040000</v>
       </c>
-      <c r="E65" s="1">
+      <c r="E66" s="1">
         <v>2449937000</v>
       </c>
-      <c r="F65" s="1">
+      <c r="F66" s="1">
         <v>2573479000</v>
       </c>
-      <c r="G65" s="1">
+      <c r="G66" s="1">
         <v>2500000000</v>
       </c>
     </row>
-    <row r="66" spans="1:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="A66" s="5" t="s">
+    <row r="67" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+      <c r="A67" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B66" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F66" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="G66" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="67" spans="1:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="A67" s="6" t="s">
+      <c r="B67" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+      <c r="A68" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B67" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="C67" s="10">
+      <c r="B68" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="C68" s="10">
         <v>7130397000</v>
       </c>
-      <c r="D67" s="10">
+      <c r="D68" s="10">
         <v>9117804000</v>
       </c>
-      <c r="E67" s="10">
+      <c r="E68" s="10">
         <v>7589716000</v>
       </c>
-      <c r="F67" s="10">
+      <c r="F68" s="10">
         <v>8932761000</v>
       </c>
-      <c r="G67" s="10">
+      <c r="G68" s="10">
         <v>10478000000</v>
       </c>
     </row>
-    <row r="68" spans="1:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="A68" s="5" t="s">
+    <row r="69" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+      <c r="A69" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B68" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C68" s="1">
+      <c r="B69" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C69" s="1">
         <v>26000</v>
       </c>
-      <c r="D68" s="1">
+      <c r="D69" s="1">
         <v>26000</v>
       </c>
-      <c r="E68" s="1">
+      <c r="E69" s="1">
         <v>60000</v>
       </c>
-      <c r="F68" s="1">
+      <c r="F69" s="1">
         <v>63000</v>
       </c>
-      <c r="G68" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="69" spans="1:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="A69" s="5" t="s">
+      <c r="G69" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+      <c r="A70" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B69" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C69" s="1">
+      <c r="B70" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C70" s="1">
         <v>-768888000</v>
       </c>
-      <c r="D69" s="1">
+      <c r="D70" s="1">
         <v>-1420991000</v>
       </c>
-      <c r="E69" s="1">
+      <c r="E70" s="1">
         <v>-6005707000</v>
       </c>
-      <c r="F69" s="1">
+      <c r="F70" s="1">
         <v>-6357741000</v>
       </c>
-      <c r="G69" s="1">
+      <c r="G70" s="1">
         <v>-5965000000</v>
       </c>
     </row>
-    <row r="70" spans="1:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="A70" s="5" t="s">
+    <row r="71" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+      <c r="A71" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B70" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C70" s="1">
+      <c r="B71" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C71" s="1">
         <v>-7912000</v>
       </c>
-      <c r="D70" s="1">
+      <c r="D71" s="1">
         <v>-4410000</v>
       </c>
-      <c r="E70" s="1">
+      <c r="E71" s="1">
         <v>2639000</v>
       </c>
-      <c r="F70" s="1">
+      <c r="F71" s="1">
         <v>-6893000</v>
       </c>
-      <c r="G70" s="1">
+      <c r="G71" s="1">
         <v>-32000000</v>
       </c>
     </row>
-    <row r="71" spans="1:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="A71" s="5" t="s">
+    <row r="72" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+      <c r="A72" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B71" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C71" s="1">
+      <c r="B72" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C72" s="1">
         <v>259466000</v>
       </c>
-      <c r="D71" s="1">
+      <c r="D72" s="1">
         <v>617690000</v>
       </c>
-      <c r="E71" s="1">
+      <c r="E72" s="1">
         <v>8904791000</v>
       </c>
-      <c r="F71" s="1">
+      <c r="F72" s="1">
         <v>11140284000</v>
       </c>
-      <c r="G71" s="1">
+      <c r="G72" s="1">
         <v>11557000000</v>
       </c>
     </row>
-    <row r="72" spans="1:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="A72" s="6" t="s">
+    <row r="73" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+      <c r="A73" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="B72" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="C72" s="10">
+      <c r="B73" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="C73" s="10">
         <v>-517308000</v>
       </c>
-      <c r="D72" s="10">
+      <c r="D73" s="10">
         <v>-807685000</v>
       </c>
-      <c r="E72" s="10">
+      <c r="E73" s="10">
         <v>2901783000</v>
       </c>
-      <c r="F72" s="10">
+      <c r="F73" s="10">
         <v>4775713000</v>
       </c>
-      <c r="G72" s="10">
+      <c r="G73" s="10">
         <v>5560000000</v>
       </c>
-      <c r="M72" s="70"/>
-    </row>
-    <row r="73" spans="1:17" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="7" t="s">
+      <c r="M73" s="58"/>
+    </row>
+    <row r="74" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="B73" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="C73" s="11">
+      <c r="B74" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="C74" s="11">
         <v>6613089000</v>
       </c>
-      <c r="D73" s="11">
+      <c r="D74" s="11">
         <v>8310119000</v>
       </c>
-      <c r="E73" s="11">
+      <c r="E74" s="11">
         <v>10491499000</v>
       </c>
-      <c r="F73" s="11">
+      <c r="F74" s="11">
         <v>13708474000</v>
       </c>
-      <c r="G73" s="11">
+      <c r="G74" s="11">
         <v>16038000000</v>
       </c>
     </row>
-    <row r="74" spans="1:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="A74" s="5" t="s">
+    <row r="75" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+      <c r="A75" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B74" s="13" t="s">
+      <c r="B75" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="C74" s="13" t="s">
+      <c r="C75" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="D74" s="13" t="s">
+      <c r="D75" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="E74" s="13" t="s">
+      <c r="E75" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="F74" s="13" t="s">
+      <c r="F75" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="G74" s="13" t="s">
+      <c r="G75" s="13" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="75" spans="1:17" ht="21" x14ac:dyDescent="0.25">
-      <c r="A75" s="4" t="s">
+    <row r="76" spans="1:13" ht="21" x14ac:dyDescent="0.25">
+      <c r="A76" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B75" s="9" t="s">
+      <c r="B76" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="C75" s="9" t="s">
+      <c r="C76" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="D75" s="9" t="s">
+      <c r="D76" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="E75" s="9" t="s">
+      <c r="E76" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="F75" s="9" t="s">
+      <c r="F76" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="G75" s="9" t="s">
+      <c r="G76" s="9" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="76" spans="1:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="A76" s="5" t="s">
+    <row r="77" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+      <c r="A77" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B76" s="1">
+      <c r="B77" s="1">
         <v>-70046000</v>
       </c>
-      <c r="C76" s="1">
+      <c r="C77" s="1">
         <v>-16860000</v>
       </c>
-      <c r="D76" s="1">
+      <c r="D77" s="1">
         <v>-674339000</v>
       </c>
-      <c r="E76" s="1">
+      <c r="E77" s="1">
         <v>-4584716000</v>
       </c>
-      <c r="F76" s="1">
+      <c r="F77" s="1">
         <v>-352034000</v>
       </c>
-      <c r="G76" s="1">
+      <c r="G77" s="1">
         <v>1893000000</v>
       </c>
     </row>
-    <row r="77" spans="1:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="A77" s="5" t="s">
+    <row r="78" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+      <c r="A78" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B77" s="1">
+      <c r="B78" s="1">
         <v>79342000</v>
       </c>
-      <c r="C77" s="1">
+      <c r="C78" s="1">
         <v>82401000</v>
       </c>
-      <c r="D77" s="1">
+      <c r="D78" s="1">
         <v>114162000</v>
       </c>
-      <c r="E77" s="1">
+      <c r="E78" s="1">
         <v>125876000</v>
       </c>
-      <c r="F77" s="1">
+      <c r="F78" s="1">
         <v>138319000</v>
       </c>
-      <c r="G77" s="1">
+      <c r="G78" s="1">
         <v>81000000</v>
       </c>
     </row>
-    <row r="78" spans="1:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="A78" s="5" t="s">
+    <row r="79" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+      <c r="A79" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B78" s="1">
+      <c r="B79" s="1">
         <v>-4180000</v>
       </c>
-      <c r="C78" s="1">
+      <c r="C79" s="1">
         <v>-5017000</v>
       </c>
-      <c r="D78" s="1">
+      <c r="D79" s="1">
         <v>-5627000</v>
       </c>
-      <c r="E78" s="1">
+      <c r="E79" s="1">
         <v>-19601000</v>
       </c>
-      <c r="F78" s="1">
+      <c r="F79" s="1">
         <v>10935000</v>
       </c>
-      <c r="G78" s="1">
+      <c r="G79" s="1">
         <v>-1000000</v>
       </c>
     </row>
-    <row r="79" spans="1:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="A79" s="5" t="s">
+    <row r="80" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+      <c r="A80" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B79" s="1">
+      <c r="B80" s="1">
         <v>38357000</v>
       </c>
-      <c r="C79" s="1">
+      <c r="C80" s="1">
         <v>53893000</v>
       </c>
-      <c r="D79" s="1">
+      <c r="D80" s="1">
         <v>97547000</v>
       </c>
-      <c r="E79" s="1">
+      <c r="E80" s="1">
         <v>3001948000</v>
       </c>
-      <c r="F79" s="1">
+      <c r="F80" s="1">
         <v>898830000</v>
       </c>
-      <c r="G79" s="1">
+      <c r="G80" s="1">
         <v>930000000</v>
       </c>
     </row>
-    <row r="80" spans="1:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="A80" s="17" t="s">
+    <row r="81" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+      <c r="A81" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="B80" s="18">
-        <f>B79/B3</f>
+      <c r="B81" s="18">
+        <f t="shared" ref="B81:G81" si="8">B80/B4</f>
         <v>1.4973137199562326E-2</v>
       </c>
-      <c r="C80" s="18">
-        <f>C79/C3</f>
+      <c r="C81" s="18">
+        <f t="shared" si="8"/>
         <v>1.4757179999370205E-2</v>
       </c>
-      <c r="D80" s="18">
-        <f>D79/D3</f>
+      <c r="D81" s="18">
+        <f t="shared" si="8"/>
         <v>2.030013491524563E-2</v>
       </c>
-      <c r="E80" s="18">
-        <f>E79/E3</f>
+      <c r="E81" s="18">
+        <f t="shared" si="8"/>
         <v>0.88862379036877337</v>
       </c>
-      <c r="F80" s="18">
-        <f>F79/F3</f>
+      <c r="F81" s="18">
+        <f t="shared" si="8"/>
         <v>0.15001101512744169</v>
       </c>
-      <c r="G80" s="18">
-        <f>G79/G3</f>
+      <c r="G81" s="18">
+        <f t="shared" si="8"/>
         <v>0.11072746755566139</v>
       </c>
-      <c r="H80" s="18"/>
-      <c r="I80" s="18"/>
-      <c r="J80" s="18"/>
-      <c r="K80" s="18"/>
-      <c r="L80" s="18"/>
-      <c r="M80" s="18"/>
-      <c r="N80" s="18"/>
-      <c r="O80" s="18"/>
-      <c r="P80" s="18"/>
-      <c r="Q80" s="18"/>
-    </row>
-    <row r="81" spans="1:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="A81" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B81" s="1">
-        <v>183202000</v>
-      </c>
-      <c r="C81" s="1">
-        <v>421029000</v>
-      </c>
-      <c r="D81" s="1">
-        <v>620382000</v>
-      </c>
-      <c r="E81" s="1">
-        <v>-284610000</v>
-      </c>
-      <c r="F81" s="1">
-        <v>637923000</v>
-      </c>
-      <c r="G81" s="1">
-        <v>319000000</v>
-      </c>
+      <c r="H81" s="18"/>
+      <c r="I81" s="18"/>
+      <c r="J81" s="18"/>
+      <c r="K81" s="18"/>
+      <c r="L81" s="18"/>
+      <c r="M81" s="18"/>
+      <c r="N81" s="18"/>
+      <c r="O81" s="18"/>
+      <c r="P81" s="18"/>
+      <c r="Q81" s="18"/>
     </row>
     <row r="82" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F82" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="G82" s="1" t="s">
-        <v>93</v>
+        <v>69</v>
+      </c>
+      <c r="B82" s="1">
+        <v>183202000</v>
+      </c>
+      <c r="C82" s="1">
+        <v>421029000</v>
+      </c>
+      <c r="D82" s="1">
+        <v>620382000</v>
+      </c>
+      <c r="E82" s="1">
+        <v>-284610000</v>
+      </c>
+      <c r="F82" s="1">
+        <v>637923000</v>
+      </c>
+      <c r="G82" s="1">
+        <v>319000000</v>
       </c>
     </row>
     <row r="83" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>34</v>
+        <v>70</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>93</v>
@@ -4915,299 +4739,299 @@
     </row>
     <row r="84" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B84" s="1">
-        <v>11758000</v>
-      </c>
-      <c r="C84" s="1">
-        <v>29837000</v>
-      </c>
-      <c r="D84" s="1">
-        <v>75716000</v>
-      </c>
-      <c r="E84" s="1">
-        <v>-73111000</v>
-      </c>
-      <c r="F84" s="1">
-        <v>39946000</v>
-      </c>
-      <c r="G84" s="1">
-        <v>20000000</v>
+        <v>34</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G84" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="85" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
       <c r="B85" s="1">
-        <v>135394000</v>
+        <v>11758000</v>
       </c>
       <c r="C85" s="1">
-        <v>145895000</v>
+        <v>29837000</v>
       </c>
       <c r="D85" s="1">
-        <v>176254000</v>
+        <v>75716000</v>
       </c>
       <c r="E85" s="1">
-        <v>-267009000</v>
+        <v>-73111000</v>
       </c>
       <c r="F85" s="1">
-        <v>495816000</v>
+        <v>39946000</v>
       </c>
       <c r="G85" s="1">
-        <v>280000000</v>
+        <v>20000000</v>
       </c>
     </row>
     <row r="86" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B86" s="1">
+        <v>135394000</v>
+      </c>
+      <c r="C86" s="1">
+        <v>145895000</v>
+      </c>
+      <c r="D86" s="1">
+        <v>176254000</v>
+      </c>
+      <c r="E86" s="1">
+        <v>-267009000</v>
+      </c>
+      <c r="F86" s="1">
+        <v>495816000</v>
+      </c>
+      <c r="G86" s="1">
+        <v>280000000</v>
+      </c>
+    </row>
+    <row r="87" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+      <c r="A87" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B86" s="1">
+      <c r="B87" s="1">
         <v>24550000</v>
       </c>
-      <c r="C86" s="1">
+      <c r="C87" s="1">
         <v>60111000</v>
       </c>
-      <c r="D86" s="1">
+      <c r="D87" s="1">
         <v>70602000</v>
       </c>
-      <c r="E86" s="1">
+      <c r="E87" s="1">
         <v>1131371000</v>
       </c>
-      <c r="F86" s="1">
+      <c r="F87" s="1">
         <v>855721000</v>
       </c>
-      <c r="G86" s="1">
+      <c r="G87" s="1">
         <v>208000000</v>
       </c>
     </row>
-    <row r="87" spans="1:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="A87" s="6" t="s">
+    <row r="88" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+      <c r="A88" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="B87" s="10">
+      <c r="B88" s="10">
         <v>251225000</v>
       </c>
-      <c r="C87" s="10">
+      <c r="C88" s="10">
         <v>595557000</v>
       </c>
-      <c r="D87" s="10">
+      <c r="D88" s="10">
         <v>222727000</v>
       </c>
-      <c r="E87" s="10">
+      <c r="E88" s="10">
         <v>-629732000</v>
       </c>
-      <c r="F87" s="10">
+      <c r="F88" s="10">
         <v>2189694000</v>
       </c>
-      <c r="G87" s="10">
+      <c r="G88" s="10">
         <v>3430000000</v>
       </c>
     </row>
-    <row r="88" spans="1:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="A88" s="5" t="s">
+    <row r="89" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+      <c r="A89" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B88" s="1">
+      <c r="B89" s="1">
         <v>-100204000</v>
       </c>
-      <c r="C88" s="1">
+      <c r="C89" s="1">
         <v>-90624000</v>
       </c>
-      <c r="D88" s="1">
+      <c r="D89" s="1">
         <v>-125452000</v>
       </c>
-      <c r="E88" s="1">
+      <c r="E89" s="1">
         <v>-37371000</v>
       </c>
-      <c r="F88" s="1">
+      <c r="F89" s="1">
         <v>-25322000</v>
       </c>
-      <c r="G88" s="1">
+      <c r="G89" s="1">
         <v>-25000000</v>
       </c>
     </row>
-    <row r="89" spans="1:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="A89" s="17" t="s">
+    <row r="90" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+      <c r="A90" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="B89" s="18">
-        <f>(-1*B88)/B3</f>
+      <c r="B90" s="18">
+        <f t="shared" ref="B90:G90" si="9">(-1*B89)/B4</f>
         <v>3.9115891230934202E-2</v>
       </c>
-      <c r="C89" s="18">
-        <f>(-1*C88)/C3</f>
+      <c r="C90" s="18">
+        <f t="shared" si="9"/>
         <v>2.4814997871020827E-2</v>
       </c>
-      <c r="D89" s="18">
-        <f>(-1*D88)/D3</f>
+      <c r="D90" s="18">
+        <f t="shared" si="9"/>
         <v>2.6107338261426746E-2</v>
       </c>
-      <c r="E89" s="18">
-        <f>(-1*E88)/E3</f>
+      <c r="E90" s="18">
+        <f t="shared" si="9"/>
         <v>1.1062403369369299E-2</v>
       </c>
-      <c r="F89" s="18">
-        <f>(-1*F88)/F3</f>
+      <c r="F90" s="18">
+        <f t="shared" si="9"/>
         <v>4.2261372284604186E-3</v>
       </c>
-      <c r="G89" s="18">
-        <f>(-1*G88)/G3</f>
+      <c r="G90" s="18">
+        <f t="shared" si="9"/>
         <v>2.9765448267650911E-3</v>
       </c>
-      <c r="H89" s="18"/>
-      <c r="I89" s="18"/>
-      <c r="J89" s="18"/>
-      <c r="K89" s="18"/>
-      <c r="L89" s="18"/>
-      <c r="M89" s="18"/>
-      <c r="N89" s="18"/>
-      <c r="O89" s="18"/>
-      <c r="P89" s="18"/>
-      <c r="Q89" s="18"/>
-    </row>
-    <row r="90" spans="1:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="A90" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B90" s="1">
-        <v>-176649000</v>
-      </c>
-      <c r="C90" s="1">
-        <v>-60150000</v>
-      </c>
-      <c r="D90" s="1">
-        <v>-400298000</v>
-      </c>
-      <c r="E90" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F90" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="G90" s="1" t="s">
-        <v>93</v>
-      </c>
+      <c r="H90" s="18"/>
+      <c r="I90" s="18"/>
+      <c r="J90" s="18"/>
+      <c r="K90" s="18"/>
+      <c r="L90" s="18"/>
+      <c r="M90" s="18"/>
+      <c r="N90" s="18"/>
+      <c r="O90" s="18"/>
+      <c r="P90" s="18"/>
+      <c r="Q90" s="18"/>
     </row>
     <row r="91" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B91" s="1">
-        <v>-1040246000</v>
+        <v>-176649000</v>
       </c>
       <c r="C91" s="1">
-        <v>-1270578000</v>
+        <v>-60150000</v>
       </c>
       <c r="D91" s="1">
-        <v>-1016155000</v>
-      </c>
-      <c r="E91" s="1">
-        <v>-3032664000</v>
-      </c>
-      <c r="F91" s="1">
-        <v>-4938188000</v>
-      </c>
-      <c r="G91" s="1">
-        <v>-4072000000</v>
+        <v>-400298000</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G91" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="92" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B92" s="1">
-        <v>528155000</v>
+        <v>-1040246000</v>
       </c>
       <c r="C92" s="1">
-        <v>756471000</v>
+        <v>-1270578000</v>
       </c>
       <c r="D92" s="1">
-        <v>1161085000</v>
+        <v>-1016155000</v>
       </c>
       <c r="E92" s="1">
-        <v>3158225000</v>
+        <v>-3032664000</v>
       </c>
       <c r="F92" s="1">
-        <v>3611055000</v>
+        <v>-4938188000</v>
       </c>
       <c r="G92" s="1">
-        <v>4071000000</v>
+        <v>-4072000000</v>
       </c>
     </row>
     <row r="93" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B93" s="1">
+        <v>528155000</v>
+      </c>
+      <c r="C93" s="1">
+        <v>756471000</v>
+      </c>
+      <c r="D93" s="1">
+        <v>1161085000</v>
+      </c>
+      <c r="E93" s="1">
+        <v>3158225000</v>
+      </c>
+      <c r="F93" s="1">
+        <v>3611055000</v>
+      </c>
+      <c r="G93" s="1">
+        <v>4071000000</v>
+      </c>
+    </row>
+    <row r="94" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+      <c r="A94" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B93" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C93" s="1">
+      <c r="B94" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C94" s="1">
         <v>-3290000</v>
       </c>
-      <c r="D93" s="1">
+      <c r="D94" s="1">
         <v>33665000</v>
       </c>
-      <c r="E93" s="1">
+      <c r="E94" s="1">
         <v>-8600000</v>
       </c>
-      <c r="F93" s="1">
+      <c r="F94" s="1">
         <v>500000</v>
       </c>
-      <c r="G93" s="1">
+      <c r="G94" s="1">
         <v>-2000000</v>
       </c>
     </row>
-    <row r="94" spans="1:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="A94" s="6" t="s">
+    <row r="95" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+      <c r="A95" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="B94" s="10">
+      <c r="B95" s="10">
         <v>-788944000</v>
       </c>
-      <c r="C94" s="10">
+      <c r="C95" s="10">
         <v>-668171000</v>
       </c>
-      <c r="D94" s="10">
+      <c r="D95" s="10">
         <v>-347155000</v>
       </c>
-      <c r="E94" s="10">
+      <c r="E95" s="10">
         <v>79590000</v>
       </c>
-      <c r="F94" s="10">
+      <c r="F95" s="10">
         <v>-1351955000</v>
       </c>
-      <c r="G94" s="10">
+      <c r="G95" s="10">
         <v>-28000000</v>
-      </c>
-    </row>
-    <row r="95" spans="1:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="A95" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D95" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E95" s="1">
-        <v>-5000000</v>
-      </c>
-      <c r="F95" s="1">
-        <v>-2207883000</v>
-      </c>
-      <c r="G95" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="96" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>93</v>
@@ -5219,10 +5043,10 @@
         <v>93</v>
       </c>
       <c r="E96" s="1">
-        <v>3650870000</v>
-      </c>
-      <c r="F96" s="1" t="s">
-        <v>93</v>
+        <v>-5000000</v>
+      </c>
+      <c r="F96" s="1">
+        <v>-2207883000</v>
       </c>
       <c r="G96" s="1" t="s">
         <v>93</v>
@@ -5230,7 +5054,7 @@
     </row>
     <row r="97" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>93</v>
@@ -5241,431 +5065,455 @@
       <c r="D97" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="E97" s="1" t="s">
-        <v>93</v>
+      <c r="E97" s="1">
+        <v>3650870000</v>
       </c>
       <c r="F97" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="G97" s="1">
-        <v>-1500000000</v>
+      <c r="G97" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="98" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B98" s="35">
-        <v>0</v>
-      </c>
-      <c r="C98" s="35">
-        <v>0</v>
-      </c>
-      <c r="D98" s="35">
-        <v>0</v>
-      </c>
-      <c r="E98" s="35">
-        <v>0</v>
-      </c>
-      <c r="F98" s="35">
-        <v>0</v>
-      </c>
-      <c r="G98" s="35">
-        <v>0</v>
+        <v>82</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G98" s="1">
+        <v>-1500000000</v>
       </c>
     </row>
     <row r="99" spans="1:17" ht="19" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B99" s="32">
+        <v>0</v>
+      </c>
+      <c r="C99" s="32">
+        <v>0</v>
+      </c>
+      <c r="D99" s="32">
+        <v>0</v>
+      </c>
+      <c r="E99" s="32">
+        <v>0</v>
+      </c>
+      <c r="F99" s="32">
+        <v>0</v>
+      </c>
+      <c r="G99" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+      <c r="A100" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B99" s="1">
+      <c r="B100" s="1">
         <v>672954000</v>
       </c>
-      <c r="C99" s="1">
+      <c r="C100" s="1">
         <v>140516000</v>
       </c>
-      <c r="D99" s="1">
+      <c r="D100" s="1">
         <v>854579000</v>
       </c>
-      <c r="E99" s="1">
+      <c r="E100" s="1">
         <v>-705056000</v>
       </c>
-      <c r="F99" s="1">
+      <c r="F100" s="1">
         <v>3639042000</v>
       </c>
-      <c r="G99" s="1">
+      <c r="G100" s="1">
         <v>811000000</v>
       </c>
     </row>
-    <row r="100" spans="1:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="A100" s="6" t="s">
+    <row r="101" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+      <c r="A101" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="B100" s="10">
+      <c r="B101" s="10">
         <v>672954000</v>
       </c>
-      <c r="C100" s="10">
+      <c r="C101" s="10">
         <v>140516000</v>
       </c>
-      <c r="D100" s="10">
+      <c r="D101" s="10">
         <v>854579000</v>
       </c>
-      <c r="E100" s="10">
+      <c r="E101" s="10">
         <v>2940814000</v>
       </c>
-      <c r="F100" s="10">
+      <c r="F101" s="10">
         <v>1431159000</v>
       </c>
-      <c r="G100" s="10">
+      <c r="G101" s="10">
         <v>-689000000</v>
       </c>
     </row>
-    <row r="101" spans="1:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="A101" s="5" t="s">
+    <row r="102" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+      <c r="A102" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B101" s="1">
+      <c r="B102" s="1">
         <v>227172000</v>
       </c>
-      <c r="C101" s="1">
+      <c r="C102" s="1">
         <v>-158919000</v>
       </c>
-      <c r="D101" s="1">
+      <c r="D102" s="1">
         <v>-25284000</v>
       </c>
-      <c r="E101" s="1">
+      <c r="E102" s="1">
         <v>134137000</v>
       </c>
-      <c r="F101" s="1">
+      <c r="F102" s="1">
         <v>-209861000</v>
       </c>
-      <c r="G101" s="1">
+      <c r="G102" s="1">
         <v>-337000000</v>
       </c>
     </row>
-    <row r="102" spans="1:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="A102" s="6" t="s">
+    <row r="103" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+      <c r="A103" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="B102" s="10">
+      <c r="B103" s="10">
         <v>362407000</v>
       </c>
-      <c r="C102" s="10">
+      <c r="C103" s="10">
         <v>-91017000</v>
       </c>
-      <c r="D102" s="10">
+      <c r="D103" s="10">
         <v>704867000</v>
       </c>
-      <c r="E102" s="10">
+      <c r="E103" s="10">
         <v>2524809000</v>
       </c>
-      <c r="F102" s="10">
+      <c r="F103" s="10">
         <v>2059037000</v>
       </c>
-      <c r="G102" s="10">
+      <c r="G103" s="10">
         <v>2376000000</v>
       </c>
     </row>
-    <row r="103" spans="1:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="A103" s="5" t="s">
+    <row r="104" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+      <c r="A104" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B103" s="1">
+      <c r="B104" s="1">
         <v>4167186000</v>
       </c>
-      <c r="C103" s="1">
+      <c r="C104" s="1">
         <v>4529593000</v>
       </c>
-      <c r="D103" s="1">
+      <c r="D104" s="1">
         <v>4438576000</v>
       </c>
-      <c r="E103" s="1">
+      <c r="E104" s="1">
         <v>5143443000</v>
       </c>
-      <c r="F103" s="1">
+      <c r="F104" s="1">
         <v>7668252000</v>
       </c>
-      <c r="G103" s="1">
+      <c r="G104" s="1">
         <v>9727000000</v>
       </c>
     </row>
-    <row r="104" spans="1:17" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="7" t="s">
+    <row r="105" spans="1:17" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="B104" s="11">
+      <c r="B105" s="11">
         <v>4529593000</v>
       </c>
-      <c r="C104" s="11">
+      <c r="C105" s="11">
         <v>4438576000</v>
       </c>
-      <c r="D104" s="11">
+      <c r="D105" s="11">
         <v>5143443000</v>
       </c>
-      <c r="E104" s="11">
+      <c r="E105" s="11">
         <v>7668252000</v>
       </c>
-      <c r="F104" s="11">
+      <c r="F105" s="11">
         <v>9727289000</v>
       </c>
-      <c r="G104" s="11">
+      <c r="G105" s="11">
         <v>12103000000</v>
       </c>
     </row>
-    <row r="105" spans="1:17" ht="20" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="17" t="s">
+    <row r="106" spans="1:17" ht="20" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B105" s="1"/>
-      <c r="C105" s="18">
-        <f>(C106/B106)-1</f>
+      <c r="B106" s="1"/>
+      <c r="C106" s="18">
+        <f>(C107/B107)-1</f>
         <v>2.3434621675131275</v>
       </c>
-      <c r="D105" s="18">
-        <f>(D106/C106)-1</f>
+      <c r="D106" s="18">
+        <f>(D107/C107)-1</f>
         <v>-0.80735067820879203</v>
       </c>
-      <c r="E105" s="18">
-        <f>(E106/D106)-1</f>
+      <c r="E106" s="18">
+        <f>(E107/D107)-1</f>
         <v>-7.8579079928039066</v>
       </c>
-      <c r="F105" s="18">
-        <f>(F106/E106)-1</f>
+      <c r="F106" s="18">
+        <f>(F107/E107)-1</f>
         <v>-4.2444345176082248</v>
       </c>
-      <c r="G105" s="18">
-        <f>(G106/F106)-1</f>
+      <c r="G106" s="18">
+        <f>(G107/F107)-1</f>
         <v>0.57320460623220049</v>
       </c>
-      <c r="H105" s="18"/>
-      <c r="I105" s="18"/>
-      <c r="J105" s="18"/>
-      <c r="K105" s="18"/>
-      <c r="L105" s="18"/>
-      <c r="M105" s="18"/>
-      <c r="N105" s="52" t="s">
+      <c r="H106" s="18"/>
+      <c r="I106" s="18"/>
+      <c r="J106" s="18"/>
+      <c r="K106" s="18"/>
+      <c r="L106" s="18"/>
+      <c r="M106" s="18"/>
+      <c r="N106" s="70" t="s">
         <v>145</v>
       </c>
-      <c r="O105" s="53"/>
-      <c r="P105" s="18"/>
-      <c r="Q105" s="18"/>
-    </row>
-    <row r="106" spans="1:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="A106" s="5" t="s">
+      <c r="O106" s="71"/>
+      <c r="P106" s="18"/>
+      <c r="Q106" s="18"/>
+    </row>
+    <row r="107" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+      <c r="A107" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B106" s="1">
+      <c r="B107" s="1">
         <v>151021000</v>
       </c>
-      <c r="C106" s="1">
+      <c r="C107" s="1">
         <v>504933000</v>
       </c>
-      <c r="D106" s="1">
+      <c r="D107" s="1">
         <v>97275000</v>
       </c>
-      <c r="E106" s="1">
+      <c r="E107" s="1">
         <v>-667103000</v>
       </c>
-      <c r="F106" s="1">
+      <c r="F107" s="1">
         <v>2164372000</v>
       </c>
-      <c r="G106" s="1">
+      <c r="G107" s="1">
         <v>3405000000</v>
       </c>
-      <c r="H106" s="69">
-        <f>G106*(1+$O$106)</f>
+      <c r="H107" s="57">
+        <f>G107*(1+$O$107)</f>
         <v>3904665499.3593912</v>
       </c>
-      <c r="I106" s="69">
-        <f>H106*(1+$O$106)</f>
+      <c r="I107" s="57">
+        <f>H107*(1+$O$107)</f>
         <v>4477654232.5660858</v>
       </c>
-      <c r="J106" s="69">
-        <f>I106*(1+$O$106)</f>
+      <c r="J107" s="57">
+        <f>I107*(1+$O$107)</f>
         <v>5134725991.1780748</v>
       </c>
-      <c r="K106" s="69">
-        <f>J106*(1+$O$106)</f>
+      <c r="K107" s="57">
+        <f>J107*(1+$O$107)</f>
         <v>5888219508.492506</v>
       </c>
-      <c r="L106" s="69">
-        <f>K106*(1+$O$106)</f>
+      <c r="L107" s="57">
+        <f>K107*(1+$O$107)</f>
         <v>6752284160.7828484</v>
       </c>
-      <c r="M106" s="54" t="s">
+      <c r="M107" s="45" t="s">
         <v>154</v>
       </c>
-      <c r="N106" s="50" t="s">
+      <c r="N107" s="43" t="s">
         <v>142</v>
       </c>
-      <c r="O106" s="73">
-        <f>(SUM(H4:L4)/5)</f>
+      <c r="O107" s="60">
+        <f>(SUM(H5:L5)/5)</f>
         <v>0.14674464004681095</v>
       </c>
     </row>
-    <row r="107" spans="1:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="H107" s="54"/>
-      <c r="I107" s="54"/>
-      <c r="J107" s="54"/>
-      <c r="K107" s="54"/>
-      <c r="L107" s="68">
-        <f>L106*(1+O107)/(O108-O107)</f>
+    <row r="108" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+      <c r="H108" s="45"/>
+      <c r="I108" s="45"/>
+      <c r="J108" s="45"/>
+      <c r="K108" s="45"/>
+      <c r="L108" s="56">
+        <f>L107*(1+O108)/(O109-O108)</f>
         <v>104720677848.7258</v>
       </c>
-      <c r="M107" s="71" t="s">
+      <c r="M108" s="59" t="s">
         <v>144</v>
       </c>
-      <c r="N107" s="64" t="s">
+      <c r="N108" s="53" t="s">
         <v>143</v>
       </c>
-      <c r="O107" s="65">
+      <c r="O108" s="54">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="108" spans="1:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="H108" s="67">
-        <f t="shared" ref="H108:J108" si="8">H107+H106</f>
+    <row r="109" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+      <c r="H109" s="56">
+        <f t="shared" ref="H109:J109" si="10">H108+H107</f>
         <v>3904665499.3593912</v>
       </c>
-      <c r="I108" s="67">
-        <f t="shared" si="8"/>
+      <c r="I109" s="56">
+        <f t="shared" si="10"/>
         <v>4477654232.5660858</v>
       </c>
-      <c r="J108" s="67">
-        <f t="shared" si="8"/>
+      <c r="J109" s="56">
+        <f t="shared" si="10"/>
         <v>5134725991.1780748</v>
       </c>
-      <c r="K108" s="67">
-        <f>K107+K106</f>
+      <c r="K109" s="56">
+        <f>K108+K107</f>
         <v>5888219508.492506</v>
       </c>
-      <c r="L108" s="67">
-        <f>L107+L106</f>
+      <c r="L109" s="56">
+        <f>L108+L107</f>
         <v>111472962009.50865</v>
       </c>
-      <c r="M108" s="72" t="s">
+      <c r="M109" s="59" t="s">
         <v>140</v>
       </c>
-      <c r="N108" s="51" t="s">
+      <c r="N109" s="44" t="s">
         <v>155</v>
       </c>
-      <c r="O108" s="66">
-        <f>N40</f>
+      <c r="O109" s="55">
+        <f>N41</f>
         <v>9.1090970828132709E-2</v>
       </c>
     </row>
-    <row r="109" spans="1:17" ht="19" x14ac:dyDescent="0.25">
-      <c r="H109" s="55" t="s">
+    <row r="110" spans="1:17" ht="19" x14ac:dyDescent="0.25">
+      <c r="H110" s="64" t="s">
         <v>156</v>
       </c>
-      <c r="I109" s="59"/>
-    </row>
-    <row r="110" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H110" s="56" t="s">
+      <c r="I110" s="65"/>
+    </row>
+    <row r="111" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H111" s="46" t="s">
         <v>146</v>
       </c>
-      <c r="I110" s="63">
-        <f>NPV(O108,H108,I108,J108,K108,L108)</f>
+      <c r="I111" s="52">
+        <f>NPV(O109,H109,I109,J109,K109,L109)</f>
         <v>87535963959.268433</v>
       </c>
     </row>
-    <row r="111" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H111" s="56" t="s">
+    <row r="112" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H112" s="46" t="s">
         <v>152</v>
       </c>
-      <c r="I111" s="63">
-        <f>G40</f>
+      <c r="I112" s="52">
+        <f>G41</f>
         <v>9622000000</v>
       </c>
     </row>
-    <row r="112" spans="1:17" ht="20" x14ac:dyDescent="0.25">
-      <c r="H112" s="56" t="s">
+    <row r="113" spans="8:9" ht="20" x14ac:dyDescent="0.25">
+      <c r="H113" s="46" t="s">
         <v>136</v>
       </c>
-      <c r="I112" s="63">
-        <f>N34</f>
+      <c r="I113" s="52">
+        <f>N35</f>
         <v>2341000000</v>
       </c>
     </row>
-    <row r="113" spans="8:9" ht="20" x14ac:dyDescent="0.25">
-      <c r="H113" s="56" t="s">
+    <row r="114" spans="8:9" ht="20" x14ac:dyDescent="0.25">
+      <c r="H114" s="46" t="s">
         <v>147</v>
       </c>
-      <c r="I113" s="63">
-        <f>I110+I111-I112</f>
+      <c r="I114" s="52">
+        <f>I111+I112-I113</f>
         <v>94816963959.268433</v>
       </c>
     </row>
-    <row r="114" spans="8:9" ht="20" x14ac:dyDescent="0.25">
-      <c r="H114" s="60" t="s">
+    <row r="115" spans="8:9" ht="20" x14ac:dyDescent="0.25">
+      <c r="H115" s="49" t="s">
         <v>153</v>
       </c>
-      <c r="I114" s="61">
+      <c r="I115" s="50">
         <v>408930000</v>
       </c>
     </row>
-    <row r="115" spans="8:9" ht="20" x14ac:dyDescent="0.25">
-      <c r="H115" s="57" t="s">
+    <row r="116" spans="8:9" ht="20" x14ac:dyDescent="0.25">
+      <c r="H116" s="47" t="s">
         <v>148</v>
       </c>
-      <c r="I115" s="76">
-        <f>I113/I114</f>
+      <c r="I116" s="63">
+        <f>I114/I115</f>
         <v>231.86600141654668</v>
       </c>
     </row>
-    <row r="116" spans="8:9" ht="20" x14ac:dyDescent="0.25">
-      <c r="H116" s="60" t="s">
+    <row r="117" spans="8:9" ht="20" x14ac:dyDescent="0.25">
+      <c r="H117" s="49" t="s">
         <v>149</v>
       </c>
-      <c r="I116" s="62">
+      <c r="I117" s="51">
         <v>126.33</v>
       </c>
     </row>
-    <row r="117" spans="8:9" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H117" s="58" t="s">
+    <row r="118" spans="8:9" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H118" s="48" t="s">
         <v>150</v>
       </c>
-      <c r="I117" s="74">
-        <f>I115/I116-1</f>
+      <c r="I118" s="61">
+        <f>I116/I117-1</f>
         <v>0.83539936211942289</v>
       </c>
     </row>
-    <row r="118" spans="8:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H118" s="58" t="s">
+    <row r="119" spans="8:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H119" s="48" t="s">
         <v>151</v>
       </c>
-      <c r="I118" s="75" t="str">
-        <f>IF(I115&gt;I116,"BUY","SELL")</f>
+      <c r="I119" s="62" t="str">
+        <f>IF(I116&gt;I117,"BUY","SELL")</f>
         <v>BUY</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="H109:I109"/>
-    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="H110:I110"/>
     <mergeCell ref="M19:N19"/>
-    <mergeCell ref="M28:N28"/>
-    <mergeCell ref="M33:N33"/>
-    <mergeCell ref="M39:N39"/>
-    <mergeCell ref="N105:O105"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="M34:N34"/>
+    <mergeCell ref="M40:N40"/>
+    <mergeCell ref="N106:O106"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" tooltip="https://roic.ai/company/ABNB" display="ROIC.AI | ABNB" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B36" r:id="rId2" tooltip="https://sec.gov" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B74" r:id="rId3" tooltip="https://sec.gov" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="C36" r:id="rId4" tooltip="https://sec.gov" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="C74" r:id="rId5" tooltip="https://sec.gov" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="D36" r:id="rId6" tooltip="https://sec.gov" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="D74" r:id="rId7" tooltip="https://sec.gov" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="E36" r:id="rId8" tooltip="https://www.sec.gov/Archives/edgar/data/1559720/000155972021000010/0001559720-21-000010-index.htm" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="E74" r:id="rId9" tooltip="https://www.sec.gov/Archives/edgar/data/1559720/000155972021000010/0001559720-21-000010-index.htm" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="F36" r:id="rId10" tooltip="https://www.sec.gov/Archives/edgar/data/1559720/000155972022000006/0001559720-22-000006-index.htm" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="F74" r:id="rId11" tooltip="https://www.sec.gov/Archives/edgar/data/1559720/000155972022000006/0001559720-22-000006-index.htm" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="G36" r:id="rId12" tooltip="https://www.sec.gov/Archives/edgar/data/1559720/000155972023000003/0001559720-23-000003-index.htm" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="G74" r:id="rId13" tooltip="https://www.sec.gov/Archives/edgar/data/1559720/000155972023000003/0001559720-23-000003-index.htm" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="B37" r:id="rId2" tooltip="https://sec.gov" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B75" r:id="rId3" tooltip="https://sec.gov" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C37" r:id="rId4" tooltip="https://sec.gov" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C75" r:id="rId5" tooltip="https://sec.gov" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="D37" r:id="rId6" tooltip="https://sec.gov" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="D75" r:id="rId7" tooltip="https://sec.gov" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="E37" r:id="rId8" tooltip="https://www.sec.gov/Archives/edgar/data/1559720/000155972021000010/0001559720-21-000010-index.htm" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E75" r:id="rId9" tooltip="https://www.sec.gov/Archives/edgar/data/1559720/000155972021000010/0001559720-21-000010-index.htm" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="F37" r:id="rId10" tooltip="https://www.sec.gov/Archives/edgar/data/1559720/000155972022000006/0001559720-22-000006-index.htm" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="F75" r:id="rId11" tooltip="https://www.sec.gov/Archives/edgar/data/1559720/000155972022000006/0001559720-22-000006-index.htm" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="G37" r:id="rId12" tooltip="https://www.sec.gov/Archives/edgar/data/1559720/000155972023000003/0001559720-23-000003-index.htm" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="G75" r:id="rId13" tooltip="https://www.sec.gov/Archives/edgar/data/1559720/000155972023000003/0001559720-23-000003-index.htm" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
     <hyperlink ref="H1" r:id="rId14" display="https://finbox.com/NASDAQGS:ABNB/explorer/revenue_proj" xr:uid="{A9B4D051-77A7-D148-BC59-D386FC73E725}"/>
+    <hyperlink ref="A3" r:id="rId15" xr:uid="{1CB1F9AA-A62F-8349-B76A-1702B2216B3A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId15"/>
+  <drawing r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>